<commit_message>
i worked part 2 sheet one and two, i will contounes later
</commit_message>
<xml_diff>
--- a/ExcelProject-Part2.xlsx
+++ b/ExcelProject-Part2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25726"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abel.shiferaw\Desktop\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abesh\Desktop\datanomics-project-exel-g3\excel-project-group-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBA026C-3F0C-46A4-896C-17FE9F1487DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CE4763BF-B0A8-4414-A2FC-5AD6FFA064F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{9C504889-49C9-40B1-AAA2-560E668D4FD1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" activeTab="1" xr2:uid="{9C504889-49C9-40B1-AAA2-560E668D4FD1}"/>
   </bookViews>
   <sheets>
     <sheet name="IF FUNCTION 01 Practice" sheetId="3" r:id="rId1"/>
@@ -21,7 +21,7 @@
     <sheet name="LEFT RIGHT MID Practice" sheetId="4" r:id="rId6"/>
     <sheet name="SUMIF Practice" sheetId="5" r:id="rId7"/>
   </sheets>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="181029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,6 +33,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -2835,7 +2837,65 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Customer Info" xfId="3" xr:uid="{5B29114F-3462-423F-BB2A-9DE6CDF9AB03}"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="23">
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="14"/>
+        <color theme="0"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <fill>
+        <patternFill patternType="solid">
+          <fgColor indexed="64"/>
+          <bgColor theme="5"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -3281,51 +3341,6 @@
       </font>
     </dxf>
     <dxf>
-      <numFmt numFmtId="19" formatCode="m/d/yyyy"/>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="14"/>
-        <color theme="0"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor indexed="64"/>
-          <bgColor theme="5"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike val="0"/>
-        <condense val="0"/>
-        <extend val="0"/>
-        <outline val="0"/>
-        <shadow val="0"/>
-        <u val="none"/>
-        <vertAlign val="baseline"/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <name val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </font>
-    </dxf>
-    <dxf>
       <font>
         <b/>
         <i val="0"/>
@@ -5226,28 +5241,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B51B56F0-2795-425A-9F95-630BE21B6E88}" name="Table2" displayName="Table2" ref="B9:D20" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B51B56F0-2795-425A-9F95-630BE21B6E88}" name="Table2" displayName="Table2" ref="B9:D20" totalsRowShown="0" headerRowDxfId="22">
   <autoFilter ref="B9:D20" xr:uid="{7EF28A09-475B-4A8C-844E-C16FB2512675}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E4E64CFB-9945-4C15-A551-B8D7EF06A537}" name="PROJECTS"/>
-    <tableColumn id="2" xr3:uid="{D1AB6584-6930-421A-AA98-1EA108A173B7}" name="PERCENTAGE" dataDxfId="19" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{7FA28F0A-B617-4825-892A-86E0AF338E4A}" name="STATUS"/>
+    <tableColumn id="2" xr3:uid="{D1AB6584-6930-421A-AA98-1EA108A173B7}" name="PERCENTAGE" dataDxfId="21" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{7FA28F0A-B617-4825-892A-86E0AF338E4A}" name="STATUS">
+      <calculatedColumnFormula>IF(C10=1, "COMPLETE", IF(C10&gt;0, "IN PROGRESS", "NOT STARTED"))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E96C941D-2748-4BFA-9175-20DE8D82015E}" name="Table28" displayName="Table28" ref="B9:E20" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E96C941D-2748-4BFA-9175-20DE8D82015E}" name="Table28" displayName="Table28" ref="B9:E20" totalsRowShown="0" headerRowDxfId="4">
   <autoFilter ref="B9:E20" xr:uid="{7EF28A09-475B-4A8C-844E-C16FB2512675}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E29561B7-DC0C-4930-BB09-664400E9B874}" name="PROJECTS"/>
-    <tableColumn id="5" xr3:uid="{7618AB37-5B72-40A8-8C15-9DE087F8CB9F}" name="DUE DATE" dataDxfId="17">
+    <tableColumn id="5" xr3:uid="{7618AB37-5B72-40A8-8C15-9DE087F8CB9F}" name="DUE DATE" dataDxfId="3">
       <calculatedColumnFormula>TODAY()+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6A55012A-8882-4F48-BB58-C8756D3DDB37}" name="PERCENTAGE" dataDxfId="16" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{894B24EC-5522-489C-992E-2FE14787EBB4}" name="STATUS">
-      <calculatedColumnFormula>IF(D10=1, "COMPLETE", IF(D10&gt;0, "IN PROGRESS", "NOT STARTED"))</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{6A55012A-8882-4F48-BB58-C8756D3DDB37}" name="PERCENTAGE" dataDxfId="2" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{894B24EC-5522-489C-992E-2FE14787EBB4}" name="STATUS" dataDxfId="1">
+      <calculatedColumnFormula>IF(D10=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D10&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D10&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5255,18 +5272,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CAEF6BB-F739-4062-A2C3-CA5AEB251540}" name="CustomerInfo" displayName="CustomerInfo" ref="A1:I92" totalsRowShown="0" dataDxfId="15" tableBorderDxfId="14" dataCellStyle="Normal_Customer Info">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CAEF6BB-F739-4062-A2C3-CA5AEB251540}" name="CustomerInfo" displayName="CustomerInfo" ref="A1:I92" totalsRowShown="0" dataDxfId="20" tableBorderDxfId="19" dataCellStyle="Normal_Customer Info">
   <autoFilter ref="A1:I92" xr:uid="{33761F1C-CD1E-4D9D-A116-776D8C10A0F3}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B21E4DF-1BE9-442C-91B6-5D982E20EAAF}" name="Customer ID" dataDxfId="13" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="2" xr3:uid="{B2303E18-46EF-4012-AFFF-2F36313522E1}" name="Company Name" dataDxfId="12" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="3" xr3:uid="{0EB485C1-E027-4E44-9816-163BE46CC5BD}" name="Contact Name" dataDxfId="11" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="5" xr3:uid="{1CD1DFB3-CC11-4FF5-BE05-FBD86F1E03DC}" name="Address" dataDxfId="10" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="6" xr3:uid="{6F40B2DC-786B-44FB-BF57-27C1F3C11A50}" name="City" dataDxfId="9" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="7" xr3:uid="{BE59FE62-06B3-4539-AAEF-4B233706746D}" name="Region" dataDxfId="8" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="8" xr3:uid="{353BC7A9-288B-485C-BD71-CE2CCA02F728}" name="Postal Code" dataDxfId="7" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="9" xr3:uid="{0F98A9A0-D426-491A-8D7E-9B7649B52B1D}" name="Country" dataDxfId="6" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="10" xr3:uid="{0B3205FC-9D0A-4B7A-9CFA-900C03ED71FB}" name="Phone" dataDxfId="5" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="1" xr3:uid="{0B21E4DF-1BE9-442C-91B6-5D982E20EAAF}" name="Customer ID" dataDxfId="18" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="2" xr3:uid="{B2303E18-46EF-4012-AFFF-2F36313522E1}" name="Company Name" dataDxfId="17" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="3" xr3:uid="{0EB485C1-E027-4E44-9816-163BE46CC5BD}" name="Contact Name" dataDxfId="16" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="5" xr3:uid="{1CD1DFB3-CC11-4FF5-BE05-FBD86F1E03DC}" name="Address" dataDxfId="15" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="6" xr3:uid="{6F40B2DC-786B-44FB-BF57-27C1F3C11A50}" name="City" dataDxfId="14" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="7" xr3:uid="{BE59FE62-06B3-4539-AAEF-4B233706746D}" name="Region" dataDxfId="13" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="8" xr3:uid="{353BC7A9-288B-485C-BD71-CE2CCA02F728}" name="Postal Code" dataDxfId="12" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="9" xr3:uid="{0F98A9A0-D426-491A-8D7E-9B7649B52B1D}" name="Country" dataDxfId="11" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="10" xr3:uid="{0B3205FC-9D0A-4B7A-9CFA-900C03ED71FB}" name="Phone" dataDxfId="10" dataCellStyle="Normal_Customer Info"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5280,7 +5297,7 @@
     <tableColumn id="2" xr3:uid="{E70E2EB2-D96E-4DF5-BC55-78AA6F7EDC88}" name="CLASS"/>
     <tableColumn id="3" xr3:uid="{E2D5E53C-F135-4D8C-AE67-B7149C399860}" name="BRANCH"/>
     <tableColumn id="4" xr3:uid="{B30C424E-11CD-470B-92EB-D5D54D805653}" name="YEAR"/>
-    <tableColumn id="5" xr3:uid="{88DAC759-628A-41A0-8715-0ED75C5C3082}" name="LEVEL CODE" dataDxfId="4">
+    <tableColumn id="5" xr3:uid="{88DAC759-628A-41A0-8715-0ED75C5C3082}" name="LEVEL CODE" dataDxfId="9">
       <calculatedColumnFormula>RIGHT(Table3[[#This Row],[TRAINING CODE]],2)</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{D9B352CE-4C3E-4CEE-89A5-9D991E3DE954}" name="LEVEL"/>
@@ -5294,7 +5311,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ABB36226-4DEB-4AA0-8FF0-40A243373A73}" name="Table4" displayName="Table4" ref="B25:C29" totalsRowShown="0">
   <autoFilter ref="B25:C29" xr:uid="{E7DC5DC1-B19A-4360-A7B3-4F8DA22B397E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3944DD68-417D-492E-BCB1-3392F6FE7BE3}" name="LEVEL CODE" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3944DD68-417D-492E-BCB1-3392F6FE7BE3}" name="LEVEL CODE" dataDxfId="8"/>
     <tableColumn id="2" xr3:uid="{39DA51BD-1853-4265-B942-70D42DC20F6D}" name="LEVEL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5308,7 +5325,7 @@
     <sortCondition ref="E25:E30"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{334C9C64-485B-403E-B9C3-88E194C4081C}" name="CLASS CODE" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{334C9C64-485B-403E-B9C3-88E194C4081C}" name="CLASS CODE" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{1E32367B-22DC-4FA7-9191-F28D5A07A69A}" name="CLASS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5322,8 +5339,8 @@
     <sortCondition ref="B7:B127"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8E09452A-7B67-4C48-855D-CFBD7204DD60}" name="MOVIE" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{C278F0A8-15A3-422C-A7A5-B3194F40A299}" name="GROSS" dataDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{8E09452A-7B67-4C48-855D-CFBD7204DD60}" name="MOVIE" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C278F0A8-15A3-422C-A7A5-B3194F40A299}" name="GROSS" dataDxfId="5" dataCellStyle="Currency"/>
     <tableColumn id="3" xr3:uid="{1EC25A71-CFAD-4981-86D7-F95D30A8DD08}" name="YEAR"/>
     <tableColumn id="4" xr3:uid="{224F018D-7E96-4C67-952B-CD3DDA3E031B}" name="RATING"/>
   </tableColumns>
@@ -5632,17 +5649,17 @@
   <dimension ref="B1:H20"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>667</v>
       </c>
@@ -5653,7 +5670,7 @@
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
     </row>
-    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>671</v>
       </c>
@@ -5664,7 +5681,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>672</v>
       </c>
@@ -5676,95 +5693,211 @@
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>673</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D11" t="str">
+        <f t="shared" ref="D11:D20" si="0">IF(C11=1, "COMPLETE", IF(C11&gt;0, "IN PROGRESS", "NOT STARTED"))</f>
+        <v>COMPLETE</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>674</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>NOT STARTED</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>675</v>
       </c>
       <c r="C13" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>676</v>
       </c>
       <c r="C14" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>677</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPLETE</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>678</v>
       </c>
       <c r="C16" s="8">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>679</v>
       </c>
       <c r="C17" s="8">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>680</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>NOT STARTED</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>681</v>
       </c>
       <c r="C19" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPLETE</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>682</v>
       </c>
       <c r="C20" s="8">
         <v>0.44</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="D10:D20">
+    <cfRule type="colorScale" priority="3">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+    <cfRule type="dataBar" priority="4">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FFFF555A"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{B9496158-AA7A-45F7-99AD-AEEDB05D37DB}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C10:C20">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF008AEF"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{BBEB7C92-4001-4D83-A921-C48328C0E60C}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+    <cfRule type="colorScale" priority="2">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FF63BE7B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FFF8696B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{B9496158-AA7A-45F7-99AD-AEEDB05D37DB}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>D10:D20</xm:sqref>
+        </x14:conditionalFormatting>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{BBEB7C92-4001-4D83-A921-C48328C0E60C}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C10:C20</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5773,18 +5906,19 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="15.33203125" customWidth="1"/>
+    <col min="2" max="3" width="15.36328125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="20.26953125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>667</v>
       </c>
@@ -5796,7 +5930,7 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
     </row>
-    <row r="9" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>671</v>
       </c>
@@ -5810,186 +5944,191 @@
         <v>683</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>672</v>
       </c>
       <c r="C10" s="14">
         <f ca="1">TODAY()+2</f>
-        <v>44899</v>
+        <v>44906</v>
       </c>
       <c r="D10" s="8">
         <v>0.88</v>
       </c>
       <c r="E10" t="str">
-        <f>IF(D10=1, "COMPLETE", IF(D10&gt;0, "IN PROGRESS", "NOT STARTED"))</f>
+        <f ca="1">IF(D10=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D10&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D10&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>673</v>
       </c>
       <c r="C11" s="14">
         <f ca="1">TODAY()+12</f>
-        <v>44909</v>
+        <v>44916</v>
       </c>
       <c r="D11" s="8">
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" ref="E11:E20" si="0">IF(D11=1, "COMPLETE", IF(D11&gt;0, "IN PROGRESS", "NOT STARTED"))</f>
+        <f ca="1">IF(D11=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D11&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D11&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>674</v>
       </c>
       <c r="C12" s="14">
         <f ca="1">TODAY()-3</f>
-        <v>44894</v>
+        <v>44901</v>
       </c>
       <c r="D12" s="8">
         <v>0</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>NOT STARTED</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+        <f ca="1">IF(D12=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D12&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D12&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
+        <v>NOT STARTED Past Due</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>675</v>
       </c>
       <c r="C13" s="14">
         <f ca="1">TODAY()+10</f>
-        <v>44907</v>
+        <v>44914</v>
       </c>
       <c r="D13" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D13=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D13&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D13&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>676</v>
       </c>
       <c r="C14" s="14">
         <f ca="1">TODAY()+1</f>
-        <v>44898</v>
+        <v>44905</v>
       </c>
       <c r="D14" s="8">
         <v>0.1</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D14=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D14&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D14&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>677</v>
       </c>
       <c r="C15" s="14">
         <f ca="1">TODAY()-5</f>
-        <v>44892</v>
+        <v>44899</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D15=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D15&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D15&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>678</v>
       </c>
       <c r="C16" s="14">
         <f ca="1">TODAY()+2</f>
-        <v>44899</v>
+        <v>44906</v>
       </c>
       <c r="D16" s="8">
         <v>0.95</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D16=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D16&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D16&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>679</v>
       </c>
       <c r="C17" s="14">
         <f ca="1">TODAY()+12</f>
-        <v>44909</v>
+        <v>44916</v>
       </c>
       <c r="D17" s="8">
         <v>0.43</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D17=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D17&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D17&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>680</v>
       </c>
       <c r="C18" s="14">
         <f ca="1">TODAY()-1</f>
-        <v>44896</v>
+        <v>44903</v>
       </c>
       <c r="D18" s="8">
         <v>0</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>NOT STARTED</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+        <f ca="1">IF(D18=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D18&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D18&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
+        <v>NOT STARTED Past Due</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>681</v>
       </c>
       <c r="C19" s="14">
-        <f t="shared" ref="C19" ca="1" si="1">TODAY()+12</f>
-        <v>44909</v>
+        <f t="shared" ref="C19" ca="1" si="0">TODAY()+12</f>
+        <v>44916</v>
       </c>
       <c r="D19" s="8">
         <v>1</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D19=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D19&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D19&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>682</v>
       </c>
       <c r="C20" s="14">
         <f ca="1">TODAY()-3</f>
-        <v>44894</v>
+        <v>44901</v>
       </c>
       <c r="D20" s="8">
         <v>0.44</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PROGRESS</v>
+        <f ca="1">IF(D20=1, "COMPLETE", (IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]],IF(D20&gt;0, "IN PROGRESS", "NOT STARTED"),_xlfn.CONCAT(IF(D20&gt;0, "IN PROGRESS", "NOT STARTED"), " Past Due"))))</f>
+        <v>IN PROGRESS Past Due</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
   </mergeCells>
+  <conditionalFormatting sqref="E10:E20">
+    <cfRule type="containsText" dxfId="0" priority="1" operator="containsText" text="Past due">
+      <formula>NOT(ISERROR(SEARCH("Past due",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="C10:C20" calculatedColumn="1"/>
@@ -6010,21 +6149,21 @@
       <selection activeCell="I11" sqref="I11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="4.90625" customWidth="1"/>
+    <col min="4" max="4" width="31.6328125" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>668</v>
       </c>
@@ -6037,7 +6176,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.5">
       <c r="B8" s="6" t="s">
         <v>659</v>
       </c>
@@ -6060,7 +6199,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.5">
       <c r="B9" s="7" t="s">
         <v>0</v>
       </c>
@@ -6077,7 +6216,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="11" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="D11" s="4" t="s">
         <v>661</v>
       </c>
@@ -6085,7 +6224,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D12" s="5"/>
       <c r="F12" s="5"/>
     </row>
@@ -6120,21 +6259,21 @@
       <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="4.90625" customWidth="1"/>
+    <col min="4" max="4" width="31.6328125" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>843</v>
       </c>
@@ -6147,7 +6286,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.5">
       <c r="B8" s="6" t="s">
         <v>659</v>
       </c>
@@ -6170,7 +6309,7 @@
         <v>666</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.5">
       <c r="B9" s="7" t="s">
         <v>23</v>
       </c>
@@ -6187,7 +6326,7 @@
       <c r="I9" s="5"/>
       <c r="J9" s="5"/>
     </row>
-    <row r="11" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="D11" s="4" t="s">
         <v>661</v>
       </c>
@@ -6195,7 +6334,7 @@
         <v>662</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="D12" s="5"/>
       <c r="F12" s="5"/>
     </row>
@@ -6230,19 +6369,19 @@
       <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1"/>
+    <col min="4" max="4" width="41.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>650</v>
       </c>
@@ -6271,7 +6410,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6300,7 +6439,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -6329,7 +6468,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6358,7 +6497,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -6387,7 +6526,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -6416,7 +6555,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -6445,7 +6584,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -6474,7 +6613,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -6503,7 +6642,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>62</v>
       </c>
@@ -6532,7 +6671,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
@@ -6561,7 +6700,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -6590,7 +6729,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>84</v>
       </c>
@@ -6619,7 +6758,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -6648,7 +6787,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -6677,7 +6816,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
@@ -6706,7 +6845,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>115</v>
       </c>
@@ -6735,7 +6874,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>121</v>
       </c>
@@ -6764,7 +6903,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>128</v>
       </c>
@@ -6793,7 +6932,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>135</v>
       </c>
@@ -6822,7 +6961,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>141</v>
       </c>
@@ -6851,7 +6990,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>149</v>
       </c>
@@ -6880,7 +7019,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>155</v>
       </c>
@@ -6909,7 +7048,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>161</v>
       </c>
@@ -6938,7 +7077,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>168</v>
       </c>
@@ -6967,7 +7106,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>175</v>
       </c>
@@ -6996,7 +7135,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>182</v>
       </c>
@@ -7025,7 +7164,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>187</v>
       </c>
@@ -7054,7 +7193,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>195</v>
       </c>
@@ -7083,7 +7222,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>203</v>
       </c>
@@ -7112,7 +7251,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>210</v>
       </c>
@@ -7141,7 +7280,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>217</v>
       </c>
@@ -7170,7 +7309,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>224</v>
       </c>
@@ -7199,7 +7338,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>233</v>
       </c>
@@ -7228,7 +7367,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>242</v>
       </c>
@@ -7257,7 +7396,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>250</v>
       </c>
@@ -7286,7 +7425,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>258</v>
       </c>
@@ -7315,7 +7454,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>265</v>
       </c>
@@ -7344,7 +7483,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>273</v>
       </c>
@@ -7373,7 +7512,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>281</v>
       </c>
@@ -7402,7 +7541,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>288</v>
       </c>
@@ -7431,7 +7570,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>295</v>
       </c>
@@ -7460,7 +7599,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>302</v>
       </c>
@@ -7489,7 +7628,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>309</v>
       </c>
@@ -7518,7 +7657,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -7547,7 +7686,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>324</v>
       </c>
@@ -7576,7 +7715,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>332</v>
       </c>
@@ -7605,7 +7744,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>340</v>
       </c>
@@ -7634,7 +7773,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>348</v>
       </c>
@@ -7663,7 +7802,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>355</v>
       </c>
@@ -7692,7 +7831,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>362</v>
       </c>
@@ -7721,7 +7860,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>370</v>
       </c>
@@ -7750,7 +7889,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>378</v>
       </c>
@@ -7779,7 +7918,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>385</v>
       </c>
@@ -7808,7 +7947,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>391</v>
       </c>
@@ -7837,7 +7976,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>396</v>
       </c>
@@ -7866,7 +8005,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>404</v>
       </c>
@@ -7895,7 +8034,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>411</v>
       </c>
@@ -7924,7 +8063,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>418</v>
       </c>
@@ -7953,7 +8092,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>424</v>
       </c>
@@ -7982,7 +8121,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>431</v>
       </c>
@@ -8011,7 +8150,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>437</v>
       </c>
@@ -8040,7 +8179,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>443</v>
       </c>
@@ -8069,7 +8208,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>449</v>
       </c>
@@ -8098,7 +8237,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>456</v>
       </c>
@@ -8127,7 +8266,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>461</v>
       </c>
@@ -8156,7 +8295,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>469</v>
       </c>
@@ -8185,7 +8324,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>476</v>
       </c>
@@ -8214,7 +8353,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>482</v>
       </c>
@@ -8243,7 +8382,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>489</v>
       </c>
@@ -8272,7 +8411,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>495</v>
       </c>
@@ -8301,7 +8440,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>503</v>
       </c>
@@ -8330,7 +8469,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>511</v>
       </c>
@@ -8359,7 +8498,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>517</v>
       </c>
@@ -8388,7 +8527,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>525</v>
       </c>
@@ -8417,7 +8556,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>531</v>
       </c>
@@ -8446,7 +8585,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>539</v>
       </c>
@@ -8475,7 +8614,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>546</v>
       </c>
@@ -8504,7 +8643,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>552</v>
       </c>
@@ -8533,7 +8672,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>560</v>
       </c>
@@ -8562,7 +8701,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>567</v>
       </c>
@@ -8591,7 +8730,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>572</v>
       </c>
@@ -8620,7 +8759,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>578</v>
       </c>
@@ -8649,7 +8788,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>585</v>
       </c>
@@ -8678,7 +8817,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>592</v>
       </c>
@@ -8707,7 +8846,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>599</v>
       </c>
@@ -8736,7 +8875,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>606</v>
       </c>
@@ -8765,7 +8904,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>613</v>
       </c>
@@ -8794,7 +8933,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>621</v>
       </c>
@@ -8823,7 +8962,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>628</v>
       </c>
@@ -8852,7 +8991,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>635</v>
       </c>
@@ -8881,7 +9020,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>642</v>
       </c>
@@ -8925,17 +9064,17 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="6" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>684</v>
       </c>
@@ -8947,7 +9086,7 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>687</v>
       </c>
@@ -8970,7 +9109,7 @@
         <v>846</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>690</v>
       </c>
@@ -8991,37 +9130,37 @@
         <v>01</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>712</v>
       </c>
     </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>711</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>713</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>714</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>716</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>699</v>
       </c>
@@ -9035,7 +9174,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B26" s="9" t="s">
         <v>691</v>
       </c>
@@ -9049,7 +9188,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B27" s="9" t="s">
         <v>692</v>
       </c>
@@ -9063,7 +9202,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B28" s="9" t="s">
         <v>693</v>
       </c>
@@ -9077,7 +9216,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:6" x14ac:dyDescent="0.35">
       <c r="B29" s="9" t="s">
         <v>698</v>
       </c>
@@ -9091,7 +9230,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:6" x14ac:dyDescent="0.35">
       <c r="E30" s="9" t="s">
         <v>702</v>
       </c>
@@ -9122,20 +9261,20 @@
   <sheetPr codeName="Sheet8"/>
   <dimension ref="B1:J127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" customWidth="1"/>
+    <col min="2" max="2" width="41.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>717</v>
       </c>
@@ -9145,7 +9284,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>733</v>
       </c>
@@ -9171,7 +9310,7 @@
         <v>842</v>
       </c>
     </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>839</v>
       </c>
@@ -9189,7 +9328,7 @@
       <c r="I8" s="13"/>
       <c r="J8" s="13"/>
     </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>814</v>
       </c>
@@ -9203,7 +9342,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>840</v>
       </c>
@@ -9217,7 +9356,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>809</v>
       </c>
@@ -9231,7 +9370,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>821</v>
       </c>
@@ -9245,7 +9384,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>729</v>
       </c>
@@ -9259,7 +9398,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>729</v>
       </c>
@@ -9273,7 +9412,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>751</v>
       </c>
@@ -9287,7 +9426,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>798</v>
       </c>
@@ -9301,7 +9440,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>761</v>
       </c>
@@ -9315,7 +9454,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>771</v>
       </c>
@@ -9329,7 +9468,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>760</v>
       </c>
@@ -9343,7 +9482,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>763</v>
       </c>
@@ -9357,7 +9496,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>813</v>
       </c>
@@ -9371,7 +9510,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>728</v>
       </c>
@@ -9385,7 +9524,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>728</v>
       </c>
@@ -9399,7 +9538,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>805</v>
       </c>
@@ -9413,7 +9552,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>762</v>
       </c>
@@ -9427,7 +9566,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>825</v>
       </c>
@@ -9441,7 +9580,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>779</v>
       </c>
@@ -9455,7 +9594,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>773</v>
       </c>
@@ -9469,7 +9608,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>725</v>
       </c>
@@ -9483,7 +9622,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>732</v>
       </c>
@@ -9497,7 +9636,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>797</v>
       </c>
@@ -9511,7 +9650,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="32" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>801</v>
       </c>
@@ -9525,7 +9664,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>746</v>
       </c>
@@ -9539,7 +9678,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>829</v>
       </c>
@@ -9553,7 +9692,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>743</v>
       </c>
@@ -9567,7 +9706,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>835</v>
       </c>
@@ -9581,7 +9720,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>827</v>
       </c>
@@ -9595,7 +9734,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>738</v>
       </c>
@@ -9609,7 +9748,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>721</v>
       </c>
@@ -9623,7 +9762,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>744</v>
       </c>
@@ -9637,7 +9776,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>739</v>
       </c>
@@ -9651,7 +9790,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>791</v>
       </c>
@@ -9665,7 +9804,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>819</v>
       </c>
@@ -9679,7 +9818,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="44" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>815</v>
       </c>
@@ -9693,7 +9832,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>826</v>
       </c>
@@ -9707,7 +9846,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>731</v>
       </c>
@@ -9721,7 +9860,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>786</v>
       </c>
@@ -9735,7 +9874,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>832</v>
       </c>
@@ -9749,7 +9888,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>828</v>
       </c>
@@ -9763,7 +9902,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>787</v>
       </c>
@@ -9777,7 +9916,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>756</v>
       </c>
@@ -9791,7 +9930,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>753</v>
       </c>
@@ -9805,7 +9944,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>737</v>
       </c>
@@ -9819,7 +9958,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>748</v>
       </c>
@@ -9833,7 +9972,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>778</v>
       </c>
@@ -9847,7 +9986,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>800</v>
       </c>
@@ -9861,7 +10000,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>810</v>
       </c>
@@ -9875,7 +10014,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>837</v>
       </c>
@@ -9889,7 +10028,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>824</v>
       </c>
@@ -9903,7 +10042,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>799</v>
       </c>
@@ -9917,7 +10056,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>782</v>
       </c>
@@ -9931,7 +10070,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>783</v>
       </c>
@@ -9945,7 +10084,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>765</v>
       </c>
@@ -9959,7 +10098,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>776</v>
       </c>
@@ -9973,7 +10112,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>670</v>
       </c>
@@ -9987,7 +10126,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>836</v>
       </c>
@@ -10001,7 +10140,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>750</v>
       </c>
@@ -10015,7 +10154,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>723</v>
       </c>
@@ -10029,7 +10168,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>722</v>
       </c>
@@ -10043,7 +10182,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>775</v>
       </c>
@@ -10057,7 +10196,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>817</v>
       </c>
@@ -10071,7 +10210,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>822</v>
       </c>
@@ -10085,7 +10224,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>730</v>
       </c>
@@ -10099,7 +10238,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>769</v>
       </c>
@@ -10113,7 +10252,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>808</v>
       </c>
@@ -10127,7 +10266,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>834</v>
       </c>
@@ -10141,7 +10280,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>742</v>
       </c>
@@ -10155,7 +10294,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>752</v>
       </c>
@@ -10169,7 +10308,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>781</v>
       </c>
@@ -10183,7 +10322,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>790</v>
       </c>
@@ -10197,7 +10336,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>785</v>
       </c>
@@ -10211,7 +10350,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>740</v>
       </c>
@@ -10225,7 +10364,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>754</v>
       </c>
@@ -10239,7 +10378,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>788</v>
       </c>
@@ -10253,7 +10392,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>741</v>
       </c>
@@ -10267,7 +10406,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>770</v>
       </c>
@@ -10281,7 +10420,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>755</v>
       </c>
@@ -10295,7 +10434,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>759</v>
       </c>
@@ -10309,7 +10448,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>767</v>
       </c>
@@ -10323,7 +10462,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>830</v>
       </c>
@@ -10337,7 +10476,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>807</v>
       </c>
@@ -10351,7 +10490,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>812</v>
       </c>
@@ -10365,7 +10504,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>766</v>
       </c>
@@ -10379,7 +10518,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>768</v>
       </c>
@@ -10393,7 +10532,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>772</v>
       </c>
@@ -10407,7 +10546,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>806</v>
       </c>
@@ -10421,7 +10560,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>833</v>
       </c>
@@ -10435,7 +10574,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>803</v>
       </c>
@@ -10449,7 +10588,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>804</v>
       </c>
@@ -10463,7 +10602,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>831</v>
       </c>
@@ -10477,7 +10616,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>780</v>
       </c>
@@ -10491,7 +10630,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>774</v>
       </c>
@@ -10505,7 +10644,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>794</v>
       </c>
@@ -10519,7 +10658,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>747</v>
       </c>
@@ -10533,7 +10672,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>719</v>
       </c>
@@ -10547,7 +10686,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>719</v>
       </c>
@@ -10561,7 +10700,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>789</v>
       </c>
@@ -10575,7 +10714,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>793</v>
       </c>
@@ -10589,7 +10728,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>823</v>
       </c>
@@ -10603,7 +10742,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>802</v>
       </c>
@@ -10617,7 +10756,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>796</v>
       </c>
@@ -10631,7 +10770,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>816</v>
       </c>
@@ -10645,7 +10784,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>745</v>
       </c>
@@ -10659,7 +10798,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>818</v>
       </c>
@@ -10673,7 +10812,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>764</v>
       </c>
@@ -10687,7 +10826,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>727</v>
       </c>
@@ -10701,7 +10840,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>724</v>
       </c>
@@ -10715,7 +10854,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>720</v>
       </c>
@@ -10729,7 +10868,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>718</v>
       </c>
@@ -10743,7 +10882,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>792</v>
       </c>
@@ -10757,7 +10896,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>784</v>
       </c>
@@ -10771,7 +10910,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>757</v>
       </c>
@@ -10785,7 +10924,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>820</v>
       </c>
@@ -10799,7 +10938,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>726</v>
       </c>
@@ -10813,7 +10952,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>811</v>
       </c>
@@ -10827,7 +10966,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>777</v>
       </c>
@@ -10841,7 +10980,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>749</v>
       </c>

</xml_diff>

<commit_message>
Work by Dawit for part two
</commit_message>
<xml_diff>
--- a/ExcelProject-Part2.xlsx
+++ b/ExcelProject-Part2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25831"/>
   <workbookPr codeName="ThisWorkbook" defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abel.shiferaw\Desktop\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\abesh\Desktop\datanomics-project-exel-g3\excel-project-group-3\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDBA026C-3F0C-46A4-896C-17FE9F1487DD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6BC984FE-06F8-44EA-9B03-05F4D3211001}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" firstSheet="4" activeTab="6" xr2:uid="{9C504889-49C9-40B1-AAA2-560E668D4FD1}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" firstSheet="2" activeTab="3" xr2:uid="{9C504889-49C9-40B1-AAA2-560E668D4FD1}"/>
   </bookViews>
   <sheets>
     <sheet name="IF FUNCTION 01 Practice" sheetId="3" r:id="rId1"/>
@@ -22,6 +22,7 @@
     <sheet name="SUMIF Practice" sheetId="5" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,6 +34,8 @@
         <xcalcf:feature name="microsoft.com:FV"/>
         <xcalcf:feature name="microsoft.com:CNMTM"/>
         <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -87,8 +90,30 @@
 </comments>
 </file>
 
+<file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+  <metadataTypes count="1">
+    <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
+  </metadataTypes>
+  <futureMetadata name="XLDAPR" count="1">
+    <bk>
+      <extLst>
+        <ext uri="{bdbb8cdc-fa1e-496e-a857-3c3f30c029c3}">
+          <xda:dynamicArrayProperties fDynamic="1" fCollapsed="0"/>
+        </ext>
+      </extLst>
+    </bk>
+  </futureMetadata>
+  <cellMetadata count="1">
+    <bk>
+      <rc t="1" v="0"/>
+    </bk>
+  </cellMetadata>
+</metadata>
+</file>
+
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1167" uniqueCount="847">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1171" uniqueCount="850">
   <si>
     <t>ALFKI</t>
   </si>
@@ -2630,6 +2655,15 @@
   </si>
   <si>
     <t>CLASS NAME</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Rating </t>
+  </si>
+  <si>
+    <t>year</t>
   </si>
 </sst>
 </file>
@@ -2640,7 +2674,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="11" x14ac:knownFonts="1">
+  <fonts count="12" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -2720,8 +2754,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="5">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -2743,6 +2784,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2801,7 +2848,7 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="3" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -2828,6 +2875,9 @@
     <xf numFmtId="0" fontId="9" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="Comma" xfId="1" builtinId="3"/>
@@ -2835,7 +2885,53 @@
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal_Customer Info" xfId="3" xr:uid="{5B29114F-3462-423F-BB2A-9DE6CDF9AB03}"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="32">
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b/>
+        <i/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF006100"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFC6EFCE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <color rgb="FF9C0006"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFC7CE"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <font>
         <b val="0"/>
@@ -2863,13 +2959,29 @@
       </fill>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="0" formatCode="General"/>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
       <font>
@@ -3263,6 +3375,9 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -5226,28 +5341,30 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B51B56F0-2795-425A-9F95-630BE21B6E88}" name="Table2" displayName="Table2" ref="B9:D20" totalsRowShown="0" headerRowDxfId="20">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{B51B56F0-2795-425A-9F95-630BE21B6E88}" name="Table2" displayName="Table2" ref="B9:D20" totalsRowShown="0" headerRowDxfId="31">
   <autoFilter ref="B9:D20" xr:uid="{7EF28A09-475B-4A8C-844E-C16FB2512675}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{E4E64CFB-9945-4C15-A551-B8D7EF06A537}" name="PROJECTS"/>
-    <tableColumn id="2" xr3:uid="{D1AB6584-6930-421A-AA98-1EA108A173B7}" name="PERCENTAGE" dataDxfId="19" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{7FA28F0A-B617-4825-892A-86E0AF338E4A}" name="STATUS"/>
+    <tableColumn id="2" xr3:uid="{D1AB6584-6930-421A-AA98-1EA108A173B7}" name="PERCENTAGE" dataDxfId="30" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{7FA28F0A-B617-4825-892A-86E0AF338E4A}" name="STATUS">
+      <calculatedColumnFormula>IF(C10=1, "COMPLETE", IF(C10&gt;0, "IN PROGRESS", "NOT STARTED"))</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E96C941D-2748-4BFA-9175-20DE8D82015E}" name="Table28" displayName="Table28" ref="B9:E20" totalsRowShown="0" headerRowDxfId="18">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E96C941D-2748-4BFA-9175-20DE8D82015E}" name="Table28" displayName="Table28" ref="B9:E20" totalsRowShown="0" headerRowDxfId="29">
   <autoFilter ref="B9:E20" xr:uid="{7EF28A09-475B-4A8C-844E-C16FB2512675}"/>
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{E29561B7-DC0C-4930-BB09-664400E9B874}" name="PROJECTS"/>
-    <tableColumn id="5" xr3:uid="{7618AB37-5B72-40A8-8C15-9DE087F8CB9F}" name="DUE DATE" dataDxfId="17">
+    <tableColumn id="5" xr3:uid="{7618AB37-5B72-40A8-8C15-9DE087F8CB9F}" name="DUE DATE" dataDxfId="28">
       <calculatedColumnFormula>TODAY()+12</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="2" xr3:uid="{6A55012A-8882-4F48-BB58-C8756D3DDB37}" name="PERCENTAGE" dataDxfId="16" dataCellStyle="Comma"/>
-    <tableColumn id="3" xr3:uid="{894B24EC-5522-489C-992E-2FE14787EBB4}" name="STATUS">
-      <calculatedColumnFormula>IF(D10=1, "COMPLETE", IF(D10&gt;0, "IN PROGRESS", "NOT STARTED"))</calculatedColumnFormula>
+    <tableColumn id="2" xr3:uid="{6A55012A-8882-4F48-BB58-C8756D3DDB37}" name="PERCENTAGE" dataDxfId="27" dataCellStyle="Comma"/>
+    <tableColumn id="3" xr3:uid="{894B24EC-5522-489C-992E-2FE14787EBB4}" name="STATUS" dataDxfId="26">
+      <calculatedColumnFormula>IF(D10=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D10&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D10&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5255,18 +5372,18 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CAEF6BB-F739-4062-A2C3-CA5AEB251540}" name="CustomerInfo" displayName="CustomerInfo" ref="A1:I92" totalsRowShown="0" dataDxfId="15" tableBorderDxfId="14" dataCellStyle="Normal_Customer Info">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{3CAEF6BB-F739-4062-A2C3-CA5AEB251540}" name="CustomerInfo" displayName="CustomerInfo" ref="A1:I92" totalsRowShown="0" dataDxfId="25" tableBorderDxfId="24" dataCellStyle="Normal_Customer Info">
   <autoFilter ref="A1:I92" xr:uid="{33761F1C-CD1E-4D9D-A116-776D8C10A0F3}"/>
   <tableColumns count="9">
-    <tableColumn id="1" xr3:uid="{0B21E4DF-1BE9-442C-91B6-5D982E20EAAF}" name="Customer ID" dataDxfId="13" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="2" xr3:uid="{B2303E18-46EF-4012-AFFF-2F36313522E1}" name="Company Name" dataDxfId="12" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="3" xr3:uid="{0EB485C1-E027-4E44-9816-163BE46CC5BD}" name="Contact Name" dataDxfId="11" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="5" xr3:uid="{1CD1DFB3-CC11-4FF5-BE05-FBD86F1E03DC}" name="Address" dataDxfId="10" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="6" xr3:uid="{6F40B2DC-786B-44FB-BF57-27C1F3C11A50}" name="City" dataDxfId="9" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="7" xr3:uid="{BE59FE62-06B3-4539-AAEF-4B233706746D}" name="Region" dataDxfId="8" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="8" xr3:uid="{353BC7A9-288B-485C-BD71-CE2CCA02F728}" name="Postal Code" dataDxfId="7" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="9" xr3:uid="{0F98A9A0-D426-491A-8D7E-9B7649B52B1D}" name="Country" dataDxfId="6" dataCellStyle="Normal_Customer Info"/>
-    <tableColumn id="10" xr3:uid="{0B3205FC-9D0A-4B7A-9CFA-900C03ED71FB}" name="Phone" dataDxfId="5" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="1" xr3:uid="{0B21E4DF-1BE9-442C-91B6-5D982E20EAAF}" name="Customer ID" dataDxfId="23" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="2" xr3:uid="{B2303E18-46EF-4012-AFFF-2F36313522E1}" name="Company Name" dataDxfId="22" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="3" xr3:uid="{0EB485C1-E027-4E44-9816-163BE46CC5BD}" name="Contact Name" dataDxfId="21" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="5" xr3:uid="{1CD1DFB3-CC11-4FF5-BE05-FBD86F1E03DC}" name="Address" dataDxfId="20" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="6" xr3:uid="{6F40B2DC-786B-44FB-BF57-27C1F3C11A50}" name="City" dataDxfId="19" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="7" xr3:uid="{BE59FE62-06B3-4539-AAEF-4B233706746D}" name="Region" dataDxfId="18" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="8" xr3:uid="{353BC7A9-288B-485C-BD71-CE2CCA02F728}" name="Postal Code" dataDxfId="17" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="9" xr3:uid="{0F98A9A0-D426-491A-8D7E-9B7649B52B1D}" name="Country" dataDxfId="16" dataCellStyle="Normal_Customer Info"/>
+    <tableColumn id="10" xr3:uid="{0B3205FC-9D0A-4B7A-9CFA-900C03ED71FB}" name="Phone" dataDxfId="15" dataCellStyle="Normal_Customer Info"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5277,14 +5394,18 @@
   <autoFilter ref="B10:H17" xr:uid="{20B99242-5724-40B5-9009-0C629037E436}"/>
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{FD1BF31B-F181-4892-8DEA-D9BDFD530C7F}" name="TRAINING CODE"/>
-    <tableColumn id="2" xr3:uid="{E70E2EB2-D96E-4DF5-BC55-78AA6F7EDC88}" name="CLASS"/>
-    <tableColumn id="3" xr3:uid="{E2D5E53C-F135-4D8C-AE67-B7149C399860}" name="BRANCH"/>
-    <tableColumn id="4" xr3:uid="{B30C424E-11CD-470B-92EB-D5D54D805653}" name="YEAR"/>
-    <tableColumn id="5" xr3:uid="{88DAC759-628A-41A0-8715-0ED75C5C3082}" name="LEVEL CODE" dataDxfId="4">
+    <tableColumn id="2" xr3:uid="{E70E2EB2-D96E-4DF5-BC55-78AA6F7EDC88}" name="CLASS" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{E2D5E53C-F135-4D8C-AE67-B7149C399860}" name="BRANCH" dataDxfId="11"/>
+    <tableColumn id="4" xr3:uid="{B30C424E-11CD-470B-92EB-D5D54D805653}" name="YEAR" dataDxfId="10"/>
+    <tableColumn id="5" xr3:uid="{88DAC759-628A-41A0-8715-0ED75C5C3082}" name="LEVEL CODE" dataDxfId="9">
       <calculatedColumnFormula>RIGHT(Table3[[#This Row],[TRAINING CODE]],2)</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="6" xr3:uid="{D9B352CE-4C3E-4CEE-89A5-9D991E3DE954}" name="LEVEL"/>
-    <tableColumn id="7" xr3:uid="{56FB84C4-842C-45D9-B9B8-56E1C80F2C98}" name="CLASS NAME"/>
+    <tableColumn id="6" xr3:uid="{D9B352CE-4C3E-4CEE-89A5-9D991E3DE954}" name="LEVEL" dataDxfId="8">
+      <calculatedColumnFormula>VLOOKUP(RIGHT(B11,2),Table4[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{56FB84C4-842C-45D9-B9B8-56E1C80F2C98}" name="CLASS NAME" dataDxfId="7">
+      <calculatedColumnFormula>VLOOKUP(LEFT(B11,2),Table46[],2,FALSE)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium3" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -5294,7 +5415,7 @@
 <table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{ABB36226-4DEB-4AA0-8FF0-40A243373A73}" name="Table4" displayName="Table4" ref="B25:C29" totalsRowShown="0">
   <autoFilter ref="B25:C29" xr:uid="{E7DC5DC1-B19A-4360-A7B3-4F8DA22B397E}"/>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{3944DD68-417D-492E-BCB1-3392F6FE7BE3}" name="LEVEL CODE" dataDxfId="3"/>
+    <tableColumn id="1" xr3:uid="{3944DD68-417D-492E-BCB1-3392F6FE7BE3}" name="LEVEL CODE" dataDxfId="14"/>
     <tableColumn id="2" xr3:uid="{39DA51BD-1853-4265-B942-70D42DC20F6D}" name="LEVEL"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5308,7 +5429,7 @@
     <sortCondition ref="E25:E30"/>
   </sortState>
   <tableColumns count="2">
-    <tableColumn id="1" xr3:uid="{334C9C64-485B-403E-B9C3-88E194C4081C}" name="CLASS CODE" dataDxfId="2"/>
+    <tableColumn id="1" xr3:uid="{334C9C64-485B-403E-B9C3-88E194C4081C}" name="CLASS CODE" dataDxfId="13"/>
     <tableColumn id="2" xr3:uid="{1E32367B-22DC-4FA7-9191-F28D5A07A69A}" name="CLASS"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5322,8 +5443,8 @@
     <sortCondition ref="B7:B127"/>
   </sortState>
   <tableColumns count="4">
-    <tableColumn id="1" xr3:uid="{8E09452A-7B67-4C48-855D-CFBD7204DD60}" name="MOVIE" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{C278F0A8-15A3-422C-A7A5-B3194F40A299}" name="GROSS" dataDxfId="0" dataCellStyle="Currency"/>
+    <tableColumn id="1" xr3:uid="{8E09452A-7B67-4C48-855D-CFBD7204DD60}" name="MOVIE" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{C278F0A8-15A3-422C-A7A5-B3194F40A299}" name="GROSS" dataDxfId="5" dataCellStyle="Currency"/>
     <tableColumn id="3" xr3:uid="{1EC25A71-CFAD-4981-86D7-F95D30A8DD08}" name="YEAR"/>
     <tableColumn id="4" xr3:uid="{224F018D-7E96-4C67-952B-CD3DDA3E031B}" name="RATING"/>
   </tableColumns>
@@ -5631,18 +5752,18 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="B1:H20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B1" sqref="B1:H1"/>
+    <sheetView topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C10" sqref="C10:C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
     <col min="3" max="3" width="18" customWidth="1"/>
-    <col min="4" max="4" width="12.5546875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:8" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>667</v>
       </c>
@@ -5653,7 +5774,7 @@
       <c r="G1" s="15"/>
       <c r="H1" s="15"/>
     </row>
-    <row r="9" spans="2:8" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:8" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>671</v>
       </c>
@@ -5664,7 +5785,7 @@
         <v>683</v>
       </c>
     </row>
-    <row r="10" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>672</v>
       </c>
@@ -5676,95 +5797,166 @@
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>673</v>
       </c>
       <c r="C11" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D11" t="str">
+        <f t="shared" ref="D11:D20" si="0">IF(C11=1, "COMPLETE", IF(C11&gt;0, "IN PROGRESS", "NOT STARTED"))</f>
+        <v>COMPLETE</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>674</v>
       </c>
       <c r="C12" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D12" t="str">
+        <f t="shared" si="0"/>
+        <v>NOT STARTED</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>675</v>
       </c>
       <c r="C13" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D13" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>676</v>
       </c>
       <c r="C14" s="8">
         <v>0.1</v>
       </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D14" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>677</v>
       </c>
       <c r="C15" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.3">
+      <c r="D15" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPLETE</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>678</v>
       </c>
       <c r="C16" s="8">
         <v>0.95</v>
       </c>
-    </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D16" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>679</v>
       </c>
       <c r="C17" s="8">
         <v>0.43</v>
       </c>
-    </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D17" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>680</v>
       </c>
       <c r="C18" s="8">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D18" t="str">
+        <f t="shared" si="0"/>
+        <v>NOT STARTED</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>681</v>
       </c>
       <c r="C19" s="8">
         <v>1</v>
       </c>
-    </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="D19" t="str">
+        <f t="shared" si="0"/>
+        <v>COMPLETE</v>
+      </c>
+    </row>
+    <row r="20" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>682</v>
       </c>
       <c r="C20" s="8">
         <v>0.44</v>
+      </c>
+      <c r="D20" t="str">
+        <f t="shared" si="0"/>
+        <v>IN PROGRESS</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:H1"/>
   </mergeCells>
+  <conditionalFormatting sqref="C10:C20">
+    <cfRule type="dataBar" priority="1">
+      <dataBar>
+        <cfvo type="min"/>
+        <cfvo type="max"/>
+        <color rgb="FF63C384"/>
+      </dataBar>
+      <extLst>
+        <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{B025F937-C7B1-47D3-B67F-A62EFF666E3E}">
+          <x14:id>{7557D70A-5DC7-48BE-9B43-13CC15A4EAC7}</x14:id>
+        </ext>
+      </extLst>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{78C0D931-6437-407d-A8EE-F0AAD7539E65}">
+      <x14:conditionalFormattings>
+        <x14:conditionalFormatting xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+          <x14:cfRule type="dataBar" id="{7557D70A-5DC7-48BE-9B43-13CC15A4EAC7}">
+            <x14:dataBar minLength="0" maxLength="100" gradient="0">
+              <x14:cfvo type="autoMin"/>
+              <x14:cfvo type="autoMax"/>
+              <x14:negativeFillColor rgb="FFFF0000"/>
+              <x14:axisColor rgb="FF000000"/>
+            </x14:dataBar>
+          </x14:cfRule>
+          <xm:sqref>C10:C20</xm:sqref>
+        </x14:conditionalFormatting>
+      </x14:conditionalFormattings>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
@@ -5773,18 +5965,18 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="B1:I20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H17" sqref="H17"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="3" width="15.33203125" customWidth="1"/>
+    <col min="2" max="3" width="15.36328125" customWidth="1"/>
     <col min="4" max="4" width="18" customWidth="1"/>
-    <col min="5" max="5" width="16.44140625" customWidth="1"/>
+    <col min="5" max="5" width="21.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:9" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>667</v>
       </c>
@@ -5796,7 +5988,7 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
     </row>
-    <row r="9" spans="2:9" ht="18" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:9" ht="18.5" x14ac:dyDescent="0.45">
       <c r="B9" s="4" t="s">
         <v>671</v>
       </c>
@@ -5810,186 +6002,194 @@
         <v>683</v>
       </c>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>672</v>
       </c>
       <c r="C10" s="14">
         <f ca="1">TODAY()+2</f>
-        <v>44899</v>
+        <v>44907</v>
       </c>
       <c r="D10" s="8">
         <v>0.88</v>
       </c>
       <c r="E10" t="str">
-        <f>IF(D10=1, "COMPLETE", IF(D10&gt;0, "IN PROGRESS", "NOT STARTED"))</f>
+        <f ca="1">IF(D10=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D10&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D10&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>673</v>
       </c>
       <c r="C11" s="14">
         <f ca="1">TODAY()+12</f>
-        <v>44909</v>
+        <v>44917</v>
       </c>
       <c r="D11" s="8">
         <v>1</v>
       </c>
       <c r="E11" t="str">
-        <f t="shared" ref="E11:E20" si="0">IF(D11=1, "COMPLETE", IF(D11&gt;0, "IN PROGRESS", "NOT STARTED"))</f>
+        <f ca="1">IF(D11=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D11&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D11&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>674</v>
       </c>
       <c r="C12" s="14">
         <f ca="1">TODAY()-3</f>
-        <v>44894</v>
+        <v>44902</v>
       </c>
       <c r="D12" s="8">
         <v>0</v>
       </c>
       <c r="E12" t="str">
-        <f t="shared" si="0"/>
-        <v>NOT STARTED</v>
-      </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+        <f ca="1">IF(D12=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D12&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D12&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
+        <v>NOT STARTED PASS DUE</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>675</v>
       </c>
       <c r="C13" s="14">
         <f ca="1">TODAY()+10</f>
-        <v>44907</v>
+        <v>44915</v>
       </c>
       <c r="D13" s="8">
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="E13" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D13=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D13&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D13&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>676</v>
       </c>
       <c r="C14" s="14">
         <f ca="1">TODAY()+1</f>
-        <v>44898</v>
+        <v>44906</v>
       </c>
       <c r="D14" s="8">
         <v>0.1</v>
       </c>
       <c r="E14" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D14=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D14&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D14&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>677</v>
       </c>
       <c r="C15" s="14">
         <f ca="1">TODAY()-5</f>
-        <v>44892</v>
+        <v>44900</v>
       </c>
       <c r="D15" s="8">
         <v>1</v>
       </c>
       <c r="E15" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D15=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D15&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D15&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="2:9" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>678</v>
       </c>
       <c r="C16" s="14">
         <f ca="1">TODAY()+2</f>
-        <v>44899</v>
+        <v>44907</v>
       </c>
       <c r="D16" s="8">
         <v>0.95</v>
       </c>
       <c r="E16" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D16=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D16&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D16&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>679</v>
       </c>
       <c r="C17" s="14">
         <f ca="1">TODAY()+12</f>
-        <v>44909</v>
+        <v>44917</v>
       </c>
       <c r="D17" s="8">
         <v>0.43</v>
       </c>
       <c r="E17" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D17=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D17&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D17&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
         <v>IN PROGRESS</v>
       </c>
     </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>680</v>
       </c>
       <c r="C18" s="14">
         <f ca="1">TODAY()-1</f>
-        <v>44896</v>
+        <v>44904</v>
       </c>
       <c r="D18" s="8">
         <v>0</v>
       </c>
       <c r="E18" t="str">
-        <f t="shared" si="0"/>
-        <v>NOT STARTED</v>
-      </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+        <f ca="1">IF(D18=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D18&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D18&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
+        <v>NOT STARTED PASS DUE</v>
+      </c>
+    </row>
+    <row r="19" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>681</v>
       </c>
       <c r="C19" s="14">
-        <f t="shared" ref="C19" ca="1" si="1">TODAY()+12</f>
-        <v>44909</v>
+        <f t="shared" ref="C19" ca="1" si="0">TODAY()+12</f>
+        <v>44917</v>
       </c>
       <c r="D19" s="8">
         <v>1</v>
       </c>
       <c r="E19" t="str">
-        <f t="shared" si="0"/>
+        <f ca="1">IF(D19=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D19&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D19&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
         <v>COMPLETE</v>
       </c>
     </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>682</v>
       </c>
       <c r="C20" s="14">
         <f ca="1">TODAY()-3</f>
-        <v>44894</v>
+        <v>44902</v>
       </c>
       <c r="D20" s="8">
         <v>0.44</v>
       </c>
       <c r="E20" t="str">
-        <f t="shared" si="0"/>
-        <v>IN PROGRESS</v>
+        <f ca="1">IF(D20=1, "COMPLETE",IF(TODAY()&lt;Table28[[#This Row],[DUE DATE]], ( IF(D20&gt;0, "IN PROGRESS", "NOT STARTED")),_xlfn.CONCAT( IF(D20&gt;0, "IN PROGRESS", "NOT STARTED")," PASS DUE")))</f>
+        <v>IN PROGRESS PASS DUE</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:I1"/>
   </mergeCells>
+  <conditionalFormatting sqref="E10:E20">
+    <cfRule type="containsText" dxfId="4" priority="1" operator="containsText" text="PASS">
+      <formula>NOT(ISERROR(SEARCH("PASS",E10)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="3" priority="2" operator="containsText" text="DUE">
+      <formula>NOT(ISERROR(SEARCH("DUE",E10)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
     <ignoredError sqref="C10:C20" calculatedColumn="1"/>
@@ -6007,24 +6207,24 @@
   <dimension ref="B1:J12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="4.90625" customWidth="1"/>
+    <col min="4" max="4" width="31.6328125" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>668</v>
       </c>
@@ -6037,7 +6237,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.5">
       <c r="B8" s="6" t="s">
         <v>659</v>
       </c>
@@ -6060,24 +6260,36 @@
         <v>666</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.5">
       <c r="B9" s="7" t="s">
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>VLOOKUP(B9,CustomerInfo[#All],2,FALSE)</f>
-        <v>Alfreds Futterkiste</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+        <v>Bottom-Dollar Markets</v>
+      </c>
+      <c r="F9" s="5" t="str">
+        <f>VLOOKUP($B$9,CustomerInfo[#All],4,0)</f>
+        <v>23 Tsawassen Blvd.</v>
+      </c>
+      <c r="G9" s="5" t="str">
+        <f>VLOOKUP($B$9,CustomerInfo[#All],5,0)</f>
+        <v>Tsawassen</v>
+      </c>
       <c r="H9" s="5" t="str">
-        <f>VLOOKUP(B9,CustomerInfo[#All],6,FALSE)</f>
-        <v/>
-      </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="11" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+        <f>VLOOKUP($B$9,CustomerInfo[#All],6,0)</f>
+        <v>BC</v>
+      </c>
+      <c r="I9" s="5" t="str">
+        <f>VLOOKUP($B$9,CustomerInfo[#All],7,0)</f>
+        <v>T2F 8M4</v>
+      </c>
+      <c r="J9" s="5" t="str">
+        <f>VLOOKUP($B$9,CustomerInfo[#All],8,0)</f>
+        <v>Canada</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="D11" s="4" t="s">
         <v>661</v>
       </c>
@@ -6085,14 +6297,25 @@
         <v>662</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D12" s="5"/>
-      <c r="F12" s="5"/>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D12" s="5" t="str">
+        <f>VLOOKUP($B$9,CustomerInfo[#All],3,1)</f>
+        <v>Elizabeth Lincoln</v>
+      </c>
+      <c r="F12" s="5" t="str">
+        <f>VLOOKUP($B$9,CustomerInfo[#All],9,1)</f>
+        <v>(604) 555-4729</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="containsText" dxfId="2" priority="1" operator="containsText" text="Canada">
+      <formula>NOT(ISERROR(SEARCH("Canada",J9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -6116,25 +6339,25 @@
   <sheetPr codeName="Sheet5"/>
   <dimension ref="B1:J12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.88671875" customWidth="1"/>
-    <col min="2" max="2" width="20.44140625" customWidth="1"/>
-    <col min="3" max="3" width="4.88671875" customWidth="1"/>
-    <col min="4" max="4" width="31.6640625" customWidth="1"/>
+    <col min="1" max="1" width="4.90625" customWidth="1"/>
+    <col min="2" max="2" width="20.453125" customWidth="1"/>
+    <col min="3" max="3" width="4.90625" customWidth="1"/>
+    <col min="4" max="4" width="31.6328125" customWidth="1"/>
     <col min="5" max="5" width="5" customWidth="1"/>
-    <col min="6" max="6" width="27.6640625" customWidth="1"/>
-    <col min="7" max="7" width="16.6640625" customWidth="1"/>
-    <col min="8" max="8" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.6328125" customWidth="1"/>
+    <col min="7" max="7" width="16.6328125" customWidth="1"/>
+    <col min="8" max="8" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="17" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="19" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:10" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>843</v>
       </c>
@@ -6147,7 +6370,7 @@
       <c r="I1" s="15"/>
       <c r="J1" s="15"/>
     </row>
-    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="8" spans="2:10" ht="21" x14ac:dyDescent="0.5">
       <c r="B8" s="6" t="s">
         <v>659</v>
       </c>
@@ -6170,24 +6393,36 @@
         <v>666</v>
       </c>
     </row>
-    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.4">
+    <row r="9" spans="2:10" ht="21" x14ac:dyDescent="0.5">
       <c r="B9" s="7" t="s">
-        <v>23</v>
+        <v>599</v>
       </c>
       <c r="D9" s="5" t="str">
         <f>INDEX(CustomerInfo[[#All],[Company Name]],MATCH('INDEX MATCH FUNCTION Practice'!$B$9,CustomerInfo[[#All],[Customer ID]],0))</f>
-        <v>Around the Horn</v>
-      </c>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
+        <v>Vins et alcools Chevalier</v>
+      </c>
+      <c r="F9" s="5" t="str">
+        <f>INDEX(CustomerInfo[Address],MATCH('INDEX MATCH FUNCTION Practice'!$B$9,CustomerInfo[[#All],[Customer ID]],0))</f>
+        <v>Adenauerallee 900</v>
+      </c>
+      <c r="G9" s="5" t="str">
+        <f>INDEX(CustomerInfo[City],MATCH('INDEX MATCH FUNCTION Practice'!$B$9,CustomerInfo[[#All],[Customer ID]],0))</f>
+        <v>Stuttgart</v>
+      </c>
       <c r="H9" s="5" t="str">
-        <f>VLOOKUP(B9,CustomerInfo[#All],6,FALSE)</f>
+        <f>INDEX(CustomerInfo[Region],MATCH('INDEX MATCH FUNCTION Practice'!$B$9,CustomerInfo[[#All],[Customer ID]],0))</f>
         <v/>
       </c>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
-    </row>
-    <row r="11" spans="2:10" ht="18" x14ac:dyDescent="0.35">
+      <c r="I9" s="5" t="str">
+        <f>INDEX(CustomerInfo[Postal Code],MATCH('INDEX MATCH FUNCTION Practice'!$B$9,CustomerInfo[[#All],[Customer ID]],0))</f>
+        <v>70563</v>
+      </c>
+      <c r="J9" s="5" t="str">
+        <f>INDEX(CustomerInfo[Country],MATCH('INDEX MATCH FUNCTION Practice'!$B$9,CustomerInfo[[#All],[Customer ID]],0))</f>
+        <v>Germany</v>
+      </c>
+    </row>
+    <row r="11" spans="2:10" ht="18.5" x14ac:dyDescent="0.45">
       <c r="D11" s="4" t="s">
         <v>661</v>
       </c>
@@ -6195,14 +6430,28 @@
         <v>662</v>
       </c>
     </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
-      <c r="D12" s="5"/>
-      <c r="F12" s="5"/>
+    <row r="12" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="D12" s="5" t="str">
+        <f>INDEX(CustomerInfo[Contact Name],MATCH('INDEX MATCH FUNCTION Practice'!$B$9,CustomerInfo[[#All],[Customer ID]],0))</f>
+        <v>Rita Müller</v>
+      </c>
+      <c r="F12" s="5" t="str">
+        <f>INDEX(CustomerInfo[Phone],MATCH('INDEX MATCH FUNCTION Practice'!$B$9,CustomerInfo[[#All],[Customer ID]],0))</f>
+        <v>0711-020361</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B1:J1"/>
   </mergeCells>
+  <conditionalFormatting sqref="J9">
+    <cfRule type="containsText" dxfId="0" priority="2" operator="containsText" text="Spain">
+      <formula>NOT(ISERROR(SEARCH("Spain",J9)))</formula>
+    </cfRule>
+    <cfRule type="containsText" dxfId="1" priority="1" operator="containsText" text="spain">
+      <formula>NOT(ISERROR(SEARCH("spain",J9)))</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
@@ -6226,23 +6475,23 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:I92"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+    <sheetView topLeftCell="A73" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="33.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.5546875" customWidth="1"/>
-    <col min="4" max="4" width="41.6640625" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="13.6640625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="25.54296875" customWidth="1"/>
+    <col min="4" max="4" width="41.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="7" width="13.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="15.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>650</v>
       </c>
@@ -6271,7 +6520,7 @@
         <v>658</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
@@ -6300,7 +6549,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>9</v>
       </c>
@@ -6329,7 +6578,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>17</v>
       </c>
@@ -6358,7 +6607,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>23</v>
       </c>
@@ -6387,7 +6636,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>31</v>
       </c>
@@ -6416,7 +6665,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>39</v>
       </c>
@@ -6445,7 +6694,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>46</v>
       </c>
@@ -6474,7 +6723,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A9" s="1" t="s">
         <v>54</v>
       </c>
@@ -6503,7 +6752,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A10" s="1" t="s">
         <v>62</v>
       </c>
@@ -6532,7 +6781,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A11" s="1" t="s">
         <v>69</v>
       </c>
@@ -6561,7 +6810,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A12" s="1" t="s">
         <v>78</v>
       </c>
@@ -6590,7 +6839,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A13" s="1" t="s">
         <v>84</v>
       </c>
@@ -6619,7 +6868,7 @@
         <v>91</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="1" t="s">
         <v>92</v>
       </c>
@@ -6648,7 +6897,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A15" s="1" t="s">
         <v>98</v>
       </c>
@@ -6677,7 +6926,7 @@
         <v>105</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A16" s="1" t="s">
         <v>106</v>
       </c>
@@ -6706,7 +6955,7 @@
         <v>114</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="1" t="s">
         <v>115</v>
       </c>
@@ -6735,7 +6984,7 @@
         <v>120</v>
       </c>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A18" s="1" t="s">
         <v>121</v>
       </c>
@@ -6764,7 +7013,7 @@
         <v>127</v>
       </c>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A19" s="1" t="s">
         <v>128</v>
       </c>
@@ -6793,7 +7042,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A20" s="1" t="s">
         <v>135</v>
       </c>
@@ -6822,7 +7071,7 @@
         <v>140</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A21" s="1" t="s">
         <v>141</v>
       </c>
@@ -6851,7 +7100,7 @@
         <v>148</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A22" s="1" t="s">
         <v>149</v>
       </c>
@@ -6880,7 +7129,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="1" t="s">
         <v>155</v>
       </c>
@@ -6909,7 +7158,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A24" s="1" t="s">
         <v>161</v>
       </c>
@@ -6938,7 +7187,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="1" t="s">
         <v>168</v>
       </c>
@@ -6967,7 +7216,7 @@
         <v>174</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A26" s="1" t="s">
         <v>175</v>
       </c>
@@ -6996,7 +7245,7 @@
         <v>181</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A27" s="1" t="s">
         <v>182</v>
       </c>
@@ -7025,7 +7274,7 @@
         <v>186</v>
       </c>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="1" t="s">
         <v>187</v>
       </c>
@@ -7054,7 +7303,7 @@
         <v>194</v>
       </c>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A29" s="1" t="s">
         <v>195</v>
       </c>
@@ -7083,7 +7332,7 @@
         <v>202</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="1" t="s">
         <v>203</v>
       </c>
@@ -7112,7 +7361,7 @@
         <v>209</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A31" s="1" t="s">
         <v>210</v>
       </c>
@@ -7141,7 +7390,7 @@
         <v>216</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A32" s="1" t="s">
         <v>217</v>
       </c>
@@ -7170,7 +7419,7 @@
         <v>223</v>
       </c>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A33" s="1" t="s">
         <v>224</v>
       </c>
@@ -7199,7 +7448,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A34" s="1" t="s">
         <v>233</v>
       </c>
@@ -7228,7 +7477,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A35" s="1" t="s">
         <v>242</v>
       </c>
@@ -7257,7 +7506,7 @@
         <v>249</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A36" s="1" t="s">
         <v>250</v>
       </c>
@@ -7286,7 +7535,7 @@
         <v>257</v>
       </c>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A37" s="1" t="s">
         <v>258</v>
       </c>
@@ -7315,7 +7564,7 @@
         <v>264</v>
       </c>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A38" s="1" t="s">
         <v>265</v>
       </c>
@@ -7344,7 +7593,7 @@
         <v>272</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A39" s="1" t="s">
         <v>273</v>
       </c>
@@ -7373,7 +7622,7 @@
         <v>280</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A40" s="1" t="s">
         <v>281</v>
       </c>
@@ -7402,7 +7651,7 @@
         <v>287</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A41" s="1" t="s">
         <v>288</v>
       </c>
@@ -7431,7 +7680,7 @@
         <v>294</v>
       </c>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A42" s="1" t="s">
         <v>295</v>
       </c>
@@ -7460,7 +7709,7 @@
         <v>301</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A43" s="1" t="s">
         <v>302</v>
       </c>
@@ -7489,7 +7738,7 @@
         <v>308</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A44" s="1" t="s">
         <v>309</v>
       </c>
@@ -7518,7 +7767,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A45" s="1" t="s">
         <v>317</v>
       </c>
@@ -7547,7 +7796,7 @@
         <v>323</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="1" t="s">
         <v>324</v>
       </c>
@@ -7576,7 +7825,7 @@
         <v>331</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A47" s="1" t="s">
         <v>332</v>
       </c>
@@ -7605,7 +7854,7 @@
         <v>339</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A48" s="1" t="s">
         <v>340</v>
       </c>
@@ -7634,7 +7883,7 @@
         <v>347</v>
       </c>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="1" t="s">
         <v>348</v>
       </c>
@@ -7663,7 +7912,7 @@
         <v>354</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A50" s="1" t="s">
         <v>355</v>
       </c>
@@ -7692,7 +7941,7 @@
         <v>361</v>
       </c>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A51" s="1" t="s">
         <v>362</v>
       </c>
@@ -7721,7 +7970,7 @@
         <v>369</v>
       </c>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A52" s="1" t="s">
         <v>370</v>
       </c>
@@ -7750,7 +7999,7 @@
         <v>377</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A53" s="1" t="s">
         <v>378</v>
       </c>
@@ -7779,7 +8028,7 @@
         <v>384</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A54" s="1" t="s">
         <v>385</v>
       </c>
@@ -7808,7 +8057,7 @@
         <v>390</v>
       </c>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="1" t="s">
         <v>391</v>
       </c>
@@ -7837,7 +8086,7 @@
         <v>395</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A56" s="1" t="s">
         <v>396</v>
       </c>
@@ -7866,7 +8115,7 @@
         <v>403</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A57" s="1" t="s">
         <v>404</v>
       </c>
@@ -7895,7 +8144,7 @@
         <v>410</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="1" t="s">
         <v>411</v>
       </c>
@@ -7924,7 +8173,7 @@
         <v>417</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A59" s="1" t="s">
         <v>418</v>
       </c>
@@ -7953,7 +8202,7 @@
         <v>423</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A60" s="1" t="s">
         <v>424</v>
       </c>
@@ -7982,7 +8231,7 @@
         <v>430</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A61" s="1" t="s">
         <v>431</v>
       </c>
@@ -8011,7 +8260,7 @@
         <v>436</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A62" s="1" t="s">
         <v>437</v>
       </c>
@@ -8040,7 +8289,7 @@
         <v>442</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A63" s="1" t="s">
         <v>443</v>
       </c>
@@ -8069,7 +8318,7 @@
         <v>448</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A64" s="1" t="s">
         <v>449</v>
       </c>
@@ -8098,7 +8347,7 @@
         <v>455</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A65" s="1" t="s">
         <v>456</v>
       </c>
@@ -8127,7 +8376,7 @@
         <v>460</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A66" s="1" t="s">
         <v>461</v>
       </c>
@@ -8156,7 +8405,7 @@
         <v>468</v>
       </c>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A67" s="1" t="s">
         <v>469</v>
       </c>
@@ -8185,7 +8434,7 @@
         <v>475</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A68" s="1" t="s">
         <v>476</v>
       </c>
@@ -8214,7 +8463,7 @@
         <v>481</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A69" s="1" t="s">
         <v>482</v>
       </c>
@@ -8243,7 +8492,7 @@
         <v>488</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A70" s="1" t="s">
         <v>489</v>
       </c>
@@ -8272,7 +8521,7 @@
         <v>494</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A71" s="1" t="s">
         <v>495</v>
       </c>
@@ -8301,7 +8550,7 @@
         <v>502</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A72" s="1" t="s">
         <v>503</v>
       </c>
@@ -8330,7 +8579,7 @@
         <v>510</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A73" s="1" t="s">
         <v>511</v>
       </c>
@@ -8359,7 +8608,7 @@
         <v>516</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A74" s="1" t="s">
         <v>517</v>
       </c>
@@ -8388,7 +8637,7 @@
         <v>524</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A75" s="1" t="s">
         <v>525</v>
       </c>
@@ -8417,7 +8666,7 @@
         <v>530</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A76" s="1" t="s">
         <v>531</v>
       </c>
@@ -8446,7 +8695,7 @@
         <v>538</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A77" s="1" t="s">
         <v>539</v>
       </c>
@@ -8475,7 +8724,7 @@
         <v>545</v>
       </c>
     </row>
-    <row r="78" spans="1:9" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" ht="29" x14ac:dyDescent="0.35">
       <c r="A78" s="1" t="s">
         <v>546</v>
       </c>
@@ -8504,7 +8753,7 @@
         <v>551</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A79" s="1" t="s">
         <v>552</v>
       </c>
@@ -8533,7 +8782,7 @@
         <v>559</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A80" s="1" t="s">
         <v>560</v>
       </c>
@@ -8562,7 +8811,7 @@
         <v>566</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A81" s="1" t="s">
         <v>567</v>
       </c>
@@ -8591,7 +8840,7 @@
         <v>571</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A82" s="1" t="s">
         <v>572</v>
       </c>
@@ -8620,7 +8869,7 @@
         <v>577</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A83" s="1" t="s">
         <v>578</v>
       </c>
@@ -8649,7 +8898,7 @@
         <v>584</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A84" s="1" t="s">
         <v>585</v>
       </c>
@@ -8678,7 +8927,7 @@
         <v>591</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A85" s="1" t="s">
         <v>592</v>
       </c>
@@ -8707,7 +8956,7 @@
         <v>598</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A86" s="1" t="s">
         <v>599</v>
       </c>
@@ -8736,7 +8985,7 @@
         <v>605</v>
       </c>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A87" s="1" t="s">
         <v>606</v>
       </c>
@@ -8765,7 +9014,7 @@
         <v>612</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A88" s="1" t="s">
         <v>613</v>
       </c>
@@ -8794,7 +9043,7 @@
         <v>620</v>
       </c>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A89" s="1" t="s">
         <v>621</v>
       </c>
@@ -8823,7 +9072,7 @@
         <v>627</v>
       </c>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="1" t="s">
         <v>628</v>
       </c>
@@ -8852,7 +9101,7 @@
         <v>634</v>
       </c>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="1" t="s">
         <v>635</v>
       </c>
@@ -8881,7 +9130,7 @@
         <v>641</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A92" s="2" t="s">
         <v>642</v>
       </c>
@@ -8921,21 +9170,23 @@
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE1FC810-1FF8-4B56-A920-8730FD8FC686}">
   <sheetPr codeName="Sheet7"/>
-  <dimension ref="B1:I30"/>
+  <dimension ref="B1:M30"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="L10" sqref="L10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="5" customWidth="1"/>
-    <col min="2" max="2" width="17.109375" customWidth="1"/>
-    <col min="3" max="3" width="14.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5546875" customWidth="1"/>
-    <col min="5" max="6" width="13.5546875" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="14.5546875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.08984375" customWidth="1"/>
+    <col min="3" max="3" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.54296875" customWidth="1"/>
+    <col min="5" max="7" width="13.54296875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:9" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:13" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>684</v>
       </c>
@@ -8947,7 +9198,7 @@
       <c r="H1" s="15"/>
       <c r="I1" s="15"/>
     </row>
-    <row r="10" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B10" t="s">
         <v>687</v>
       </c>
@@ -8970,58 +9221,213 @@
         <v>846</v>
       </c>
     </row>
-    <row r="11" spans="2:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>690</v>
       </c>
-      <c r="C11" t="str">
+      <c r="C11" s="3" t="str">
         <f>LEFT(B11,2)</f>
         <v>EX</v>
       </c>
-      <c r="D11" t="str">
+      <c r="D11" s="3" t="str">
         <f>MID(B11,4,2)</f>
         <v>SF</v>
       </c>
-      <c r="E11" t="str">
+      <c r="E11" s="3" t="str">
         <f>MID(B11,7,4)</f>
         <v>2019</v>
       </c>
-      <c r="F11" t="str">
+      <c r="F11" s="3" t="str">
         <f>RIGHT(Table3[[#This Row],[TRAINING CODE]],2)</f>
         <v>01</v>
       </c>
-    </row>
-    <row r="12" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="G11" t="str">
+        <f>VLOOKUP(RIGHT(B11,2),Table4[],2,FALSE)</f>
+        <v>BEGINNER</v>
+      </c>
+      <c r="H11" t="str">
+        <f>VLOOKUP(LEFT(B11,2),Table46[],2,FALSE)</f>
+        <v>EXCEL</v>
+      </c>
+    </row>
+    <row r="12" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>712</v>
       </c>
-    </row>
-    <row r="13" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C12" s="3" t="str">
+        <f>LEFT(B12,2)</f>
+        <v>WD</v>
+      </c>
+      <c r="D12" s="3" t="str">
+        <f>MID(B12,4,2)</f>
+        <v>SL</v>
+      </c>
+      <c r="E12" s="3" t="str">
+        <f>MID(B12,7,4)</f>
+        <v>2019</v>
+      </c>
+      <c r="F12" s="3" t="str">
+        <f>RIGHT(B12,2)</f>
+        <v>01</v>
+      </c>
+      <c r="G12" t="str">
+        <f>VLOOKUP(RIGHT(B12,2),Table4[],2,FALSE)</f>
+        <v>BEGINNER</v>
+      </c>
+      <c r="H12" t="str">
+        <f>VLOOKUP(LEFT(B12,2),Table46[],2,FALSE)</f>
+        <v>WORD</v>
+      </c>
+    </row>
+    <row r="13" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>711</v>
       </c>
-    </row>
-    <row r="14" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C13" s="3" t="str">
+        <f t="shared" ref="C13:C17" si="0">LEFT(B13,2)</f>
+        <v>EX</v>
+      </c>
+      <c r="D13" s="3" t="str">
+        <f t="shared" ref="D13:D17" si="1">MID(B13,4,2)</f>
+        <v>SL</v>
+      </c>
+      <c r="E13" s="3" t="str">
+        <f t="shared" ref="E13:E17" si="2">MID(B13,7,4)</f>
+        <v>2020</v>
+      </c>
+      <c r="F13" s="3" t="str">
+        <f t="shared" ref="F13:F17" si="3">RIGHT(B13,2)</f>
+        <v>02</v>
+      </c>
+      <c r="G13" t="str">
+        <f>VLOOKUP(RIGHT(B13,2),Table4[],2,FALSE)</f>
+        <v>INTERMEDIATE</v>
+      </c>
+      <c r="H13" t="str">
+        <f>VLOOKUP(LEFT(B13,2),Table46[],2,FALSE)</f>
+        <v>EXCEL</v>
+      </c>
+    </row>
+    <row r="14" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>713</v>
       </c>
-    </row>
-    <row r="15" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C14" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>AC</v>
+      </c>
+      <c r="D14" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>LA</v>
+      </c>
+      <c r="E14" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>2020</v>
+      </c>
+      <c r="F14" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="G14" t="str">
+        <f>VLOOKUP(RIGHT(B14,2),Table4[],2,FALSE)</f>
+        <v>BEGINNER</v>
+      </c>
+      <c r="H14" t="str">
+        <f>VLOOKUP(LEFT(B14,2),Table46[],2,FALSE)</f>
+        <v>ACCESS</v>
+      </c>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>714</v>
       </c>
-    </row>
-    <row r="16" spans="2:9" x14ac:dyDescent="0.3">
+      <c r="C15" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>EX</v>
+      </c>
+      <c r="D15" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>SL</v>
+      </c>
+      <c r="E15" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>2020</v>
+      </c>
+      <c r="F15" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>03</v>
+      </c>
+      <c r="G15" t="str">
+        <f>VLOOKUP(RIGHT(B15,2),Table4[],2,FALSE)</f>
+        <v>ADVANCED</v>
+      </c>
+      <c r="H15" t="str">
+        <f>VLOOKUP(LEFT(B15,2),Table46[],2,FALSE)</f>
+        <v>EXCEL</v>
+      </c>
+      <c r="M15" t="s">
+        <v>847</v>
+      </c>
+    </row>
+    <row r="16" spans="2:13" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>715</v>
       </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C16" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>OU</v>
+      </c>
+      <c r="D16" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>SF</v>
+      </c>
+      <c r="E16" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>2019</v>
+      </c>
+      <c r="F16" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>01</v>
+      </c>
+      <c r="G16" t="str">
+        <f>VLOOKUP(RIGHT(B16,2),Table4[],2,FALSE)</f>
+        <v>BEGINNER</v>
+      </c>
+      <c r="H16" t="str">
+        <f>VLOOKUP(LEFT(B16,2),Table46[],2,FALSE)</f>
+        <v>OUTLOOK</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>716</v>
       </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="C17" s="3" t="str">
+        <f t="shared" si="0"/>
+        <v>PP</v>
+      </c>
+      <c r="D17" s="3" t="str">
+        <f t="shared" si="1"/>
+        <v>SL</v>
+      </c>
+      <c r="E17" s="3" t="str">
+        <f t="shared" si="2"/>
+        <v>2019</v>
+      </c>
+      <c r="F17" s="3" t="str">
+        <f t="shared" si="3"/>
+        <v>02</v>
+      </c>
+      <c r="G17" t="str">
+        <f>VLOOKUP(RIGHT(B17,2),Table4[],2,FALSE)</f>
+        <v>INTERMEDIATE</v>
+      </c>
+      <c r="H17" t="str">
+        <f>VLOOKUP(LEFT(B17,2),Table46[],2,FALSE)</f>
+        <v>POWERPOINT</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>699</v>
       </c>
@@ -9035,7 +9441,7 @@
         <v>688</v>
       </c>
     </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B26" s="9" t="s">
         <v>691</v>
       </c>
@@ -9049,7 +9455,7 @@
         <v>708</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B27" s="9" t="s">
         <v>692</v>
       </c>
@@ -9063,7 +9469,7 @@
         <v>705</v>
       </c>
     </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B28" s="9" t="s">
         <v>693</v>
       </c>
@@ -9077,7 +9483,7 @@
         <v>710</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B29" s="9" t="s">
         <v>698</v>
       </c>
@@ -9091,7 +9497,7 @@
         <v>707</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="30" spans="2:8" x14ac:dyDescent="0.35">
       <c r="E30" s="9" t="s">
         <v>702</v>
       </c>
@@ -9120,22 +9526,30 @@
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{70583DB1-6205-46E3-8FFF-BF3768A835FC}">
   <sheetPr codeName="Sheet8"/>
-  <dimension ref="B1:J127"/>
+  <dimension ref="B1:Q127"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A7" sqref="A7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="5.5546875" customWidth="1"/>
-    <col min="2" max="2" width="41.109375" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.88671875" customWidth="1"/>
-    <col min="7" max="7" width="10.88671875" customWidth="1"/>
-    <col min="9" max="9" width="16.33203125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="5.54296875" customWidth="1"/>
+    <col min="2" max="2" width="41.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9.90625" customWidth="1"/>
+    <col min="7" max="7" width="10.90625" customWidth="1"/>
+    <col min="9" max="9" width="16.36328125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="14.08984375" bestFit="1" customWidth="1"/>
+    <col min="11" max="12" width="8.7265625" customWidth="1"/>
+    <col min="13" max="13" width="6.453125" style="17" customWidth="1"/>
+    <col min="14" max="14" width="4.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="2.81640625" style="17" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="8.7265625" style="17" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="3.54296875" style="17" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:10" ht="23.4" x14ac:dyDescent="0.45">
+    <row r="1" spans="2:15" ht="23.5" x14ac:dyDescent="0.55000000000000004">
       <c r="B1" s="15" t="s">
         <v>717</v>
       </c>
@@ -9145,7 +9559,7 @@
       <c r="F1" s="15"/>
       <c r="G1" s="15"/>
     </row>
-    <row r="7" spans="2:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B7" t="s">
         <v>733</v>
       </c>
@@ -9170,8 +9584,15 @@
       <c r="J7" s="12" t="s">
         <v>842</v>
       </c>
-    </row>
-    <row r="8" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="M7" s="18" t="s">
+        <v>848</v>
+      </c>
+      <c r="N7" s="16" t="s">
+        <v>849</v>
+      </c>
+      <c r="O7" s="18"/>
+    </row>
+    <row r="8" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B8" s="11" t="s">
         <v>839</v>
       </c>
@@ -9184,12 +9605,33 @@
       <c r="E8" t="s">
         <v>838</v>
       </c>
-      <c r="G8" s="5"/>
-      <c r="H8" s="5"/>
-      <c r="I8" s="13"/>
-      <c r="J8" s="13"/>
-    </row>
-    <row r="9" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="G8" s="5" t="s">
+        <v>838</v>
+      </c>
+      <c r="H8" s="5">
+        <v>2004</v>
+      </c>
+      <c r="I8" s="13">
+        <f>SUMIFS(Table6[GROSS],Table6[RATING],G8,Table6[YEAR],H8)</f>
+        <v>370782930</v>
+      </c>
+      <c r="J8" s="5">
+        <f>COUNTIF(Table6[RATING],G8)</f>
+        <v>45</v>
+      </c>
+      <c r="M8" s="18" t="str" cm="1">
+        <f t="array" ref="M8:M11">_xlfn.UNIQUE(Table6[RATING])</f>
+        <v>R</v>
+      </c>
+      <c r="N8" s="18" cm="1">
+        <f t="array" ref="N8:N46">_xlfn._xlws.SORT(_xlfn.UNIQUE(Table6[YEAR]))</f>
+        <v>1939</v>
+      </c>
+      <c r="O8" s="18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B9" t="s">
         <v>814</v>
       </c>
@@ -9202,8 +9644,17 @@
       <c r="E9" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="10" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="M9" s="18" t="str">
+        <v>G</v>
+      </c>
+      <c r="N9" s="18">
+        <v>1973</v>
+      </c>
+      <c r="O9" s="18">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B10" s="11" t="s">
         <v>840</v>
       </c>
@@ -9216,8 +9667,17 @@
       <c r="E10" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="11" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="M10" s="18" t="str">
+        <v>PG</v>
+      </c>
+      <c r="N10" s="18">
+        <v>1977</v>
+      </c>
+      <c r="O10" s="18">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="11" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B11" t="s">
         <v>809</v>
       </c>
@@ -9230,8 +9690,17 @@
       <c r="E11" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="12" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="M11" s="18" t="str">
+        <v>PG-13</v>
+      </c>
+      <c r="N11" s="18">
+        <v>1982</v>
+      </c>
+      <c r="O11" s="18">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="12" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B12" t="s">
         <v>821</v>
       </c>
@@ -9244,8 +9713,15 @@
       <c r="E12" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="13" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="M12" s="18"/>
+      <c r="N12" s="18">
+        <v>1983</v>
+      </c>
+      <c r="O12" s="18">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="13" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B13" t="s">
         <v>729</v>
       </c>
@@ -9258,8 +9734,14 @@
       <c r="E13" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="14" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="N13" s="17">
+        <v>1984</v>
+      </c>
+      <c r="O13" s="17">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="14" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B14" t="s">
         <v>729</v>
       </c>
@@ -9272,8 +9754,14 @@
       <c r="E14" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="15" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="N14" s="17">
+        <v>1987</v>
+      </c>
+      <c r="O14" s="17">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="15" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B15" t="s">
         <v>751</v>
       </c>
@@ -9286,8 +9774,14 @@
       <c r="E15" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="16" spans="2:10" x14ac:dyDescent="0.3">
+      <c r="N15" s="17">
+        <v>1988</v>
+      </c>
+      <c r="O15" s="17">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="16" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B16" t="s">
         <v>798</v>
       </c>
@@ -9300,8 +9794,14 @@
       <c r="E16" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="17" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N16" s="17">
+        <v>1990</v>
+      </c>
+      <c r="O16" s="17">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="17" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B17" t="s">
         <v>761</v>
       </c>
@@ -9314,8 +9814,14 @@
       <c r="E17" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="18" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N17" s="17">
+        <v>1991</v>
+      </c>
+      <c r="O17" s="17">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="18" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B18" t="s">
         <v>771</v>
       </c>
@@ -9328,8 +9834,14 @@
       <c r="E18" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="19" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N18" s="17">
+        <v>1992</v>
+      </c>
+      <c r="O18" s="17">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B19" t="s">
         <v>760</v>
       </c>
@@ -9342,8 +9854,14 @@
       <c r="E19" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="20" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N19" s="17">
+        <v>1993</v>
+      </c>
+      <c r="O19" s="17">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="20" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B20" t="s">
         <v>763</v>
       </c>
@@ -9356,8 +9874,14 @@
       <c r="E20" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="21" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N20" s="17">
+        <v>1994</v>
+      </c>
+      <c r="O20" s="17">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B21" t="s">
         <v>813</v>
       </c>
@@ -9370,8 +9894,18 @@
       <c r="E21" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="22" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="H21" t="e">
+        <f>SUMIFS(Table6[GROSS],Table6[[#All],[RATING]],G8,Table6[YEAR],H8)</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="N21" s="17">
+        <v>1995</v>
+      </c>
+      <c r="O21" s="17">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B22" t="s">
         <v>728</v>
       </c>
@@ -9384,8 +9918,14 @@
       <c r="E22" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="23" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N22" s="17">
+        <v>1996</v>
+      </c>
+      <c r="O22" s="17">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B23" t="s">
         <v>728</v>
       </c>
@@ -9398,8 +9938,14 @@
       <c r="E23" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="24" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N23" s="17">
+        <v>1997</v>
+      </c>
+      <c r="O23" s="17">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="24" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B24" t="s">
         <v>805</v>
       </c>
@@ -9412,8 +9958,14 @@
       <c r="E24" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="25" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N24" s="17">
+        <v>1998</v>
+      </c>
+      <c r="O24" s="17">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B25" t="s">
         <v>762</v>
       </c>
@@ -9426,8 +9978,14 @@
       <c r="E25" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="26" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N25" s="17">
+        <v>1999</v>
+      </c>
+      <c r="O25" s="17">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="26" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B26" t="s">
         <v>825</v>
       </c>
@@ -9440,8 +9998,14 @@
       <c r="E26" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="27" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N26" s="17">
+        <v>2000</v>
+      </c>
+      <c r="O26" s="17">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="27" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B27" t="s">
         <v>779</v>
       </c>
@@ -9454,8 +10018,14 @@
       <c r="E27" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="28" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N27" s="17">
+        <v>2001</v>
+      </c>
+      <c r="O27" s="17">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="28" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B28" t="s">
         <v>773</v>
       </c>
@@ -9468,8 +10038,14 @@
       <c r="E28" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="29" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N28" s="17">
+        <v>2002</v>
+      </c>
+      <c r="O28" s="17">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B29" t="s">
         <v>725</v>
       </c>
@@ -9482,8 +10058,14 @@
       <c r="E29" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="30" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N29" s="17">
+        <v>2003</v>
+      </c>
+      <c r="O29" s="17">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="30" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B30" t="s">
         <v>732</v>
       </c>
@@ -9496,8 +10078,14 @@
       <c r="E30" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="31" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N30" s="17">
+        <v>2004</v>
+      </c>
+      <c r="O30" s="17">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="31" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B31" t="s">
         <v>797</v>
       </c>
@@ -9510,8 +10098,14 @@
       <c r="E31" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="32" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N31" s="17">
+        <v>2005</v>
+      </c>
+      <c r="O31" s="17">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="32" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B32" t="s">
         <v>801</v>
       </c>
@@ -9524,8 +10118,14 @@
       <c r="E32" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N32" s="17">
+        <v>2006</v>
+      </c>
+      <c r="O32" s="17">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B33" t="s">
         <v>746</v>
       </c>
@@ -9538,8 +10138,14 @@
       <c r="E33" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N33" s="17">
+        <v>2007</v>
+      </c>
+      <c r="O33" s="17">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="34" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B34" t="s">
         <v>829</v>
       </c>
@@ -9552,8 +10158,14 @@
       <c r="E34" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N34" s="17">
+        <v>2008</v>
+      </c>
+      <c r="O34" s="17">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="35" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B35" t="s">
         <v>743</v>
       </c>
@@ -9566,8 +10178,14 @@
       <c r="E35" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N35" s="17">
+        <v>2009</v>
+      </c>
+      <c r="O35" s="17">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="36" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B36" t="s">
         <v>835</v>
       </c>
@@ -9580,8 +10198,14 @@
       <c r="E36" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N36" s="17">
+        <v>2010</v>
+      </c>
+      <c r="O36" s="17">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="37" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B37" t="s">
         <v>827</v>
       </c>
@@ -9594,8 +10218,14 @@
       <c r="E37" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N37" s="17">
+        <v>2011</v>
+      </c>
+      <c r="O37" s="17">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="38" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B38" t="s">
         <v>738</v>
       </c>
@@ -9608,8 +10238,14 @@
       <c r="E38" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N38" s="17">
+        <v>2012</v>
+      </c>
+      <c r="O38" s="17">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="39" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B39" t="s">
         <v>721</v>
       </c>
@@ -9622,8 +10258,14 @@
       <c r="E39" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N39" s="17">
+        <v>2013</v>
+      </c>
+      <c r="O39" s="17">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="40" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B40" t="s">
         <v>744</v>
       </c>
@@ -9636,8 +10278,14 @@
       <c r="E40" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N40" s="17">
+        <v>2014</v>
+      </c>
+      <c r="O40" s="17">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B41" t="s">
         <v>739</v>
       </c>
@@ -9650,8 +10298,14 @@
       <c r="E41" t="s">
         <v>758</v>
       </c>
-    </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N41" s="17">
+        <v>2015</v>
+      </c>
+      <c r="O41" s="17">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="42" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B42" t="s">
         <v>791</v>
       </c>
@@ -9664,8 +10318,14 @@
       <c r="E42" t="s">
         <v>795</v>
       </c>
-    </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N42" s="17">
+        <v>2016</v>
+      </c>
+      <c r="O42" s="17">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="43" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B43" t="s">
         <v>819</v>
       </c>
@@ -9678,8 +10338,14 @@
       <c r="E43" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="44" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N43" s="17">
+        <v>2017</v>
+      </c>
+      <c r="O43" s="17">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="44" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B44" t="s">
         <v>815</v>
       </c>
@@ -9692,8 +10358,14 @@
       <c r="E44" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N44" s="17">
+        <v>2018</v>
+      </c>
+      <c r="O44" s="17">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="45" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B45" t="s">
         <v>826</v>
       </c>
@@ -9706,8 +10378,14 @@
       <c r="E45" t="s">
         <v>838</v>
       </c>
-    </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N45" s="17">
+        <v>2019</v>
+      </c>
+      <c r="O45" s="17">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="46" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B46" t="s">
         <v>731</v>
       </c>
@@ -9720,8 +10398,14 @@
       <c r="E46" t="s">
         <v>736</v>
       </c>
-    </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.3">
+      <c r="N46" s="17">
+        <v>2020</v>
+      </c>
+      <c r="O46" s="17">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B47" t="s">
         <v>786</v>
       </c>
@@ -9735,7 +10419,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="48" spans="2:15" x14ac:dyDescent="0.35">
       <c r="B48" t="s">
         <v>832</v>
       </c>
@@ -9749,7 +10433,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="49" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="49" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B49" t="s">
         <v>828</v>
       </c>
@@ -9763,7 +10447,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="50" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="50" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B50" t="s">
         <v>787</v>
       </c>
@@ -9777,7 +10461,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="51" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="51" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B51" t="s">
         <v>756</v>
       </c>
@@ -9791,7 +10475,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="52" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="52" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B52" t="s">
         <v>753</v>
       </c>
@@ -9805,7 +10489,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="53" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="53" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B53" t="s">
         <v>737</v>
       </c>
@@ -9819,7 +10503,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="54" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="54" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B54" t="s">
         <v>748</v>
       </c>
@@ -9833,7 +10517,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="55" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="55" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B55" t="s">
         <v>778</v>
       </c>
@@ -9847,7 +10531,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="56" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="56" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B56" t="s">
         <v>800</v>
       </c>
@@ -9861,7 +10545,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="57" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="57" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B57" t="s">
         <v>810</v>
       </c>
@@ -9875,7 +10559,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="58" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="58" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B58" t="s">
         <v>837</v>
       </c>
@@ -9889,7 +10573,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="59" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="59" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B59" t="s">
         <v>824</v>
       </c>
@@ -9903,7 +10587,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="60" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="60" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B60" t="s">
         <v>799</v>
       </c>
@@ -9917,7 +10601,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="61" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="61" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B61" t="s">
         <v>782</v>
       </c>
@@ -9931,7 +10615,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="62" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="62" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B62" t="s">
         <v>783</v>
       </c>
@@ -9945,7 +10629,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="63" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="63" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B63" t="s">
         <v>765</v>
       </c>
@@ -9959,7 +10643,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="64" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="64" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B64" t="s">
         <v>776</v>
       </c>
@@ -9973,7 +10657,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B65" t="s">
         <v>670</v>
       </c>
@@ -9987,7 +10671,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B66" t="s">
         <v>836</v>
       </c>
@@ -10001,7 +10685,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B67" t="s">
         <v>750</v>
       </c>
@@ -10015,7 +10699,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B68" t="s">
         <v>723</v>
       </c>
@@ -10029,7 +10713,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B69" t="s">
         <v>722</v>
       </c>
@@ -10043,7 +10727,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B70" t="s">
         <v>775</v>
       </c>
@@ -10057,7 +10741,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B71" t="s">
         <v>817</v>
       </c>
@@ -10071,7 +10755,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B72" t="s">
         <v>822</v>
       </c>
@@ -10085,7 +10769,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B73" t="s">
         <v>730</v>
       </c>
@@ -10099,7 +10783,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B74" t="s">
         <v>769</v>
       </c>
@@ -10113,7 +10797,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B75" t="s">
         <v>808</v>
       </c>
@@ -10127,7 +10811,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B76" t="s">
         <v>834</v>
       </c>
@@ -10141,7 +10825,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B77" t="s">
         <v>742</v>
       </c>
@@ -10155,7 +10839,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B78" t="s">
         <v>752</v>
       </c>
@@ -10169,7 +10853,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B79" t="s">
         <v>781</v>
       </c>
@@ -10183,7 +10867,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B80" t="s">
         <v>790</v>
       </c>
@@ -10197,7 +10881,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="81" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B81" t="s">
         <v>785</v>
       </c>
@@ -10211,7 +10895,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="82" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="82" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B82" t="s">
         <v>740</v>
       </c>
@@ -10225,7 +10909,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="83" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B83" t="s">
         <v>754</v>
       </c>
@@ -10239,7 +10923,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="84" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="84" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B84" t="s">
         <v>788</v>
       </c>
@@ -10253,7 +10937,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="85" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="85" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B85" t="s">
         <v>741</v>
       </c>
@@ -10267,7 +10951,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="86" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="86" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B86" t="s">
         <v>770</v>
       </c>
@@ -10281,7 +10965,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="87" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="87" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B87" t="s">
         <v>755</v>
       </c>
@@ -10295,7 +10979,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="88" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="88" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B88" t="s">
         <v>759</v>
       </c>
@@ -10309,7 +10993,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="89" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="89" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B89" t="s">
         <v>767</v>
       </c>
@@ -10323,7 +11007,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="90" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="90" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B90" t="s">
         <v>830</v>
       </c>
@@ -10337,7 +11021,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="91" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="91" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B91" t="s">
         <v>807</v>
       </c>
@@ -10351,7 +11035,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="92" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="92" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B92" t="s">
         <v>812</v>
       </c>
@@ -10365,7 +11049,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="93" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="93" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B93" t="s">
         <v>766</v>
       </c>
@@ -10379,7 +11063,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="94" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="94" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B94" t="s">
         <v>768</v>
       </c>
@@ -10393,7 +11077,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="95" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="95" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B95" t="s">
         <v>772</v>
       </c>
@@ -10407,7 +11091,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="96" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="96" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B96" t="s">
         <v>806</v>
       </c>
@@ -10421,7 +11105,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="97" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="97" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B97" t="s">
         <v>833</v>
       </c>
@@ -10435,7 +11119,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="98" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="98" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B98" t="s">
         <v>803</v>
       </c>
@@ -10449,7 +11133,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="99" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="99" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B99" t="s">
         <v>804</v>
       </c>
@@ -10463,7 +11147,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="100" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="100" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B100" t="s">
         <v>831</v>
       </c>
@@ -10477,7 +11161,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="101" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="101" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B101" t="s">
         <v>780</v>
       </c>
@@ -10491,7 +11175,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="102" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="102" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B102" t="s">
         <v>774</v>
       </c>
@@ -10505,7 +11189,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="103" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="103" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B103" t="s">
         <v>794</v>
       </c>
@@ -10519,7 +11203,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="104" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="104" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B104" t="s">
         <v>747</v>
       </c>
@@ -10533,7 +11217,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="105" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="105" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B105" t="s">
         <v>719</v>
       </c>
@@ -10547,7 +11231,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="106" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="106" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B106" t="s">
         <v>719</v>
       </c>
@@ -10561,7 +11245,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="107" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="107" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B107" t="s">
         <v>789</v>
       </c>
@@ -10575,7 +11259,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="108" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="108" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B108" t="s">
         <v>793</v>
       </c>
@@ -10589,7 +11273,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="109" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="109" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B109" t="s">
         <v>823</v>
       </c>
@@ -10603,7 +11287,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="110" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="110" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B110" t="s">
         <v>802</v>
       </c>
@@ -10617,7 +11301,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="111" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="111" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B111" t="s">
         <v>796</v>
       </c>
@@ -10631,7 +11315,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="112" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="112" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B112" t="s">
         <v>816</v>
       </c>
@@ -10645,7 +11329,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="113" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="113" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B113" t="s">
         <v>745</v>
       </c>
@@ -10659,7 +11343,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="114" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="114" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B114" t="s">
         <v>818</v>
       </c>
@@ -10673,7 +11357,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="115" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="115" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B115" t="s">
         <v>764</v>
       </c>
@@ -10687,7 +11371,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="116" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="116" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B116" t="s">
         <v>727</v>
       </c>
@@ -10701,7 +11385,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="117" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="117" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B117" t="s">
         <v>724</v>
       </c>
@@ -10715,7 +11399,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="118" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="118" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B118" t="s">
         <v>720</v>
       </c>
@@ -10729,7 +11413,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="119" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="119" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B119" t="s">
         <v>718</v>
       </c>
@@ -10743,7 +11427,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="120" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="120" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B120" t="s">
         <v>792</v>
       </c>
@@ -10757,7 +11441,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="121" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="121" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B121" t="s">
         <v>784</v>
       </c>
@@ -10771,7 +11455,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="122" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="122" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B122" t="s">
         <v>757</v>
       </c>
@@ -10785,7 +11469,7 @@
         <v>758</v>
       </c>
     </row>
-    <row r="123" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="123" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B123" t="s">
         <v>820</v>
       </c>
@@ -10799,7 +11483,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="124" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="124" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B124" t="s">
         <v>726</v>
       </c>
@@ -10813,7 +11497,7 @@
         <v>736</v>
       </c>
     </row>
-    <row r="125" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="125" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B125" t="s">
         <v>811</v>
       </c>
@@ -10827,7 +11511,7 @@
         <v>838</v>
       </c>
     </row>
-    <row r="126" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="126" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B126" t="s">
         <v>777</v>
       </c>
@@ -10841,7 +11525,7 @@
         <v>795</v>
       </c>
     </row>
-    <row r="127" spans="2:5" x14ac:dyDescent="0.3">
+    <row r="127" spans="2:5" x14ac:dyDescent="0.35">
       <c r="B127" t="s">
         <v>749</v>
       </c>
@@ -10860,6 +11544,17 @@
     <mergeCell ref="B1:G1"/>
   </mergeCells>
   <phoneticPr fontId="10" type="noConversion"/>
+  <dataValidations count="3">
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G8" xr:uid="{F987B19D-FE25-4C08-8943-8E424026E531}">
+      <formula1>$M$8:$M$11</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="G18" xr:uid="{0C308AA8-BF57-4416-BA01-19CB6CF5DEC0}">
+      <formula1>_xlfn.UNIQUE($E$8:$E$27)</formula1>
+    </dataValidation>
+    <dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="H8" xr:uid="{0700D02E-0F67-435A-AEA0-DF9D6B2DFC5C}">
+      <formula1>$N$8:$N$46</formula1>
+    </dataValidation>
+  </dataValidations>
   <hyperlinks>
     <hyperlink ref="D53" r:id="rId1" display="https://www.boxofficemojo.com/year/2018/?ref_=bo_cso_table_1" xr:uid="{40A87CB3-DEE4-41E3-92CE-A890D8DC5CAB}"/>
     <hyperlink ref="D106" r:id="rId2" display="https://www.boxofficemojo.com/year/2019/?ref_=bo_cso_table_2" xr:uid="{DE2185E5-10B5-4B13-82FD-AE34A5659279}"/>

</xml_diff>